<commit_message>
1. Merge HEX and Crc16_modbus function. 2. Update Script Template version on 20191212
</commit_message>
<xml_diff>
--- a/branches/Woodpecker_All/Woodpecker/Woodpecker/Reference/Schedule/Woodpecker_Script Template(With RC).xlsx
+++ b/branches/Woodpecker_All/Woodpecker/Woodpecker/Reference/Schedule/Woodpecker_Script Template(With RC).xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\auo\rd\ASC\RRVC00\ADQAA0\[2] Smart Test\Woodpecker\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\auo\rd\ASC\ADQA00\ADQAA0\[2] Smart Test\Woodpecker\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,6 +25,7 @@
     <definedName name="_Pin">List!$D$11:$D$22</definedName>
     <definedName name="Cmd_list">List!$A$2:$A$96</definedName>
     <definedName name="COM">List!$D$2:$D$8</definedName>
+    <definedName name="CRC">List!$L$2:$L$3</definedName>
     <definedName name="switch">List!$H$8:$H$17</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -1236,7 +1237,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>_savelog</t>
+    <t>CRC16_Modbus</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1362,7 +1363,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1414,12 +1415,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1607,7 +1602,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1694,9 +1689,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1880,10 +1872,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1891,12 +1880,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1922,6 +1928,125 @@
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2270,16 +2395,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="85" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="86" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="87" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="88" t="s">
         <v>241</v>
       </c>
       <c r="E1" s="15" t="s">
@@ -2294,16 +2419,16 @@
       <c r="H1" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="89" t="s">
         <v>244</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="J1" s="90" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
-      <c r="B2" s="46"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -2315,7 +2440,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
-      <c r="B3" s="46"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -2327,7 +2452,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
-      <c r="B4" s="46"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -2339,7 +2464,7 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
-      <c r="B5" s="46"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -2351,7 +2476,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
-      <c r="B6" s="46"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -2363,7 +2488,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
-      <c r="B7" s="46"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -2375,7 +2500,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="46"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -2387,7 +2512,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
-      <c r="B9" s="46"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -2399,7 +2524,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
-      <c r="B10" s="46"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -2411,7 +2536,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
-      <c r="B11" s="46"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -2423,7 +2548,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
-      <c r="B12" s="46"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -2435,7 +2560,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
-      <c r="B13" s="46"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -2447,7 +2572,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="46"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -2459,7 +2584,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
-      <c r="B15" s="46"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -2471,7 +2596,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
-      <c r="B16" s="46"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -2483,7 +2608,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
-      <c r="B17" s="46"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2495,7 +2620,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
-      <c r="B18" s="46"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -2507,7 +2632,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
-      <c r="B19" s="46"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -2519,7 +2644,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
-      <c r="B20" s="46"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -2531,7 +2656,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
-      <c r="B21" s="46"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -2543,7 +2668,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
-      <c r="B22" s="46"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -2555,7 +2680,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
-      <c r="B23" s="46"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -2567,7 +2692,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
-      <c r="B24" s="46"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -2579,7 +2704,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
-      <c r="B25" s="46"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
@@ -2591,7 +2716,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
-      <c r="B26" s="46"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="23"/>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
@@ -2603,7 +2728,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
-      <c r="B27" s="46"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="23"/>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
@@ -2615,7 +2740,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
-      <c r="B28" s="46"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="23"/>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
@@ -2627,7 +2752,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
-      <c r="B29" s="46"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="23"/>
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
@@ -2639,7 +2764,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
-      <c r="B30" s="46"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
@@ -2651,7 +2776,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
-      <c r="B31" s="46"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
@@ -2665,46 +2790,46 @@
   <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B31">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>IF(OR(A2="_HEX",A2="_ascii",A2="_shot",A2="_rc_start",A2="_rc_stop",A2="_cmd",A2="_DOS",A2="_Pin",A2="_quantum",A2="_astro",A2="_dektec"),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C31">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="19" priority="7">
       <formula>IF(OR(A2="_HEX",A2="_ascii",A2="_shot",A2="_rc_start",A2="_rc_stop",A2="_cmd",A2="_DOS",A2="_IO_Output",A2="_IO_Input",A2="_Pin",A2="_keyword",A2="_quantum",A2="_astro",A2="_dektec"),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D31">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>IF(OR(A2="",A2="_HEX",A2="_ascii",A2="_Pin"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E31">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="17" priority="5">
       <formula>IF(OR(A2="",A2="_astro",A2="_quantum",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>IF(OR(A2="",A2="_quantum",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>IF(OR(A2="",A2="_HEX",A2="_ascii",A2="_DOS",A2="_Pin",A2="_keyword",A2="_dektec",A2="_audio_debounce"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>IF(OR(A2="",A2="_ascii",A2="_cmd",A2="_dektec"),0,1)</formula>
+    <cfRule type="expression" dxfId="13" priority="2">
+      <formula>IF(OR(A2="",A2="_ascii",A2="_HEX",A2="_cmd",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>IF(OR(G2="_save",G2="_clear"),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A31">
       <formula1>Cmd_list</formula1>
@@ -2712,11 +2837,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G31">
       <formula1>IF(OR(A2="_HEX",A2="_ascii"),_log,IF(E2="Front tyre",_ABS_front,IF(E2="Rare tyre",_ABS_rare,IF(E2="Other",_ABS_other,IF(A2="_Temperature",_temp,IF(OR(A2="_Pin",A2="_keyword"),_P_cmd,""))))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H31">
-      <formula1>IF(A2="_ascii",_NEL,IF(A2="_FuncKey",_NEL,IF(A2="_cmd",switch,IF(A2="_dektec",_dektec,""))))</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H31">
+      <formula1>IF(A3="_ascii",_NEL,IF(A3="_FuncKey",_NEL,IF(A3="_cmd",switch,IF(A3="_dektec",_dektec,""))))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31">
       <formula1>IF(OR(A2="_HEX",A2="_ascii",A2="_FuncKey"),COM,IF(A2="_Pin",_Pin,""))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+      <formula1>IF(A2="_ascii",_NEL,IF(A2="_FuncKey",_NEL,IF(A2="_cmd",switch,IF(A2="_dektec",_dektec,IF(A2="_HEX",CRC,"")))))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2730,7 +2858,7 @@
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2752,7 +2880,7 @@
       <c r="C1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="92" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="16" t="s">
@@ -2785,7 +2913,9 @@
         <v>47</v>
       </c>
       <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
+      <c r="L2" s="24" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2794,17 +2924,17 @@
       <c r="D3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="91" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>42</v>
       </c>
       <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
+      <c r="L3" s="26"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="25" t="s">
@@ -2841,7 +2971,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="47" t="s">
         <v>177</v>
       </c>
       <c r="D7" s="25" t="s">
@@ -2849,23 +2979,23 @@
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="48" t="s">
         <v>178</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="H8" s="83" t="s">
+      <c r="H8" s="82" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>179</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
-      <c r="H9" s="84" t="s">
+      <c r="H9" s="83" t="s">
         <v>3</v>
       </c>
       <c r="K9" s="24">
@@ -2873,12 +3003,12 @@
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="46" t="s">
         <v>180</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
-      <c r="H10" s="84" t="s">
+      <c r="H10" s="83" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="25">
@@ -2886,17 +3016,17 @@
       </c>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="49" t="s">
         <v>181</v>
       </c>
       <c r="C11" s="21"/>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="84" t="s">
+      <c r="H11" s="83" t="s">
         <v>6</v>
       </c>
       <c r="K11" s="25">
@@ -2909,13 +3039,13 @@
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="84" t="s">
+      <c r="H12" s="83" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="25">
@@ -2923,20 +3053,20 @@
       </c>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>183</v>
       </c>
       <c r="B13" s="24">
         <v>1</v>
       </c>
       <c r="C13" s="21"/>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="84" t="s">
+      <c r="H13" s="83" t="s">
         <v>7</v>
       </c>
       <c r="K13" s="25">
@@ -2951,14 +3081,14 @@
         <v>2</v>
       </c>
       <c r="C14" s="21"/>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="42" t="s">
         <v>56</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="84" t="s">
+      <c r="H14" s="83" t="s">
         <v>236</v>
       </c>
       <c r="K14" s="25">
@@ -2973,14 +3103,14 @@
         <v>3</v>
       </c>
       <c r="C15" s="21"/>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="42" t="s">
         <v>57</v>
       </c>
       <c r="E15" s="21"/>
       <c r="G15" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="84" t="s">
+      <c r="H15" s="83" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="25">
@@ -2995,14 +3125,14 @@
         <v>4</v>
       </c>
       <c r="C16" s="21"/>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="42" t="s">
         <v>58</v>
       </c>
       <c r="E16" s="21"/>
       <c r="G16" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="84" t="s">
+      <c r="H16" s="83" t="s">
         <v>235</v>
       </c>
       <c r="K16" s="25">
@@ -3017,14 +3147,14 @@
         <v>5</v>
       </c>
       <c r="C17" s="21"/>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="42" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="21"/>
       <c r="G17" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="85" t="s">
+      <c r="H17" s="84" t="s">
         <v>8</v>
       </c>
       <c r="K17" s="25">
@@ -3039,7 +3169,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="21"/>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="42" t="s">
         <v>60</v>
       </c>
       <c r="E18" s="21"/>
@@ -3058,11 +3188,11 @@
         <v>7</v>
       </c>
       <c r="C19" s="21"/>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="42" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="21"/>
-      <c r="H19" s="32"/>
+      <c r="H19" s="31"/>
       <c r="K19" s="25">
         <v>30</v>
       </c>
@@ -3074,11 +3204,11 @@
       <c r="B20" s="25">
         <v>8</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="42" t="s">
         <v>62</v>
       </c>
       <c r="E20" s="21"/>
-      <c r="H20" s="51" t="s">
+      <c r="H20" s="50" t="s">
         <v>90</v>
       </c>
       <c r="K20" s="25">
@@ -3092,7 +3222,7 @@
       <c r="B21" s="25">
         <v>9</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H21" s="28" t="s">
@@ -3109,7 +3239,7 @@
       <c r="B22" s="26">
         <v>10</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="43" t="s">
         <v>64</v>
       </c>
       <c r="K22" s="25">
@@ -3516,8 +3646,8 @@
   <dimension ref="A1:R118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3579,170 +3709,172 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="69" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="68" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="96" t="s">
+        <v>254</v>
+      </c>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="69" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68" t="s">
         <v>233</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="34" t="s">
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="I3" s="70"/>
-      <c r="J3" s="71"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="69" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="68" t="s">
         <v>233</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="74" t="s">
+      <c r="E4" s="71"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="73" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="20"/>
-      <c r="J4" s="31"/>
+      <c r="J4" s="30"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="31"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>247</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
       <c r="I6" s="21"/>
-      <c r="J6" s="76"/>
+      <c r="J6" s="75"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="78"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="77"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="57" t="s">
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="56" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="21"/>
-      <c r="J8" s="76"/>
+      <c r="J8" s="75"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="57" t="s">
+      <c r="A9" s="54"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="56" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="21"/>
-      <c r="J9" s="76"/>
+      <c r="J9" s="75"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="57" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="56" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="21"/>
-      <c r="J10" s="76"/>
+      <c r="J10" s="75"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="57" t="s">
+      <c r="A11" s="54"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="56" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="21"/>
-      <c r="J11" s="76"/>
+      <c r="J11" s="75"/>
     </row>
     <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="57" t="s">
+      <c r="A12" s="54"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="56" t="s">
         <v>10</v>
       </c>
       <c r="I12" s="21"/>
-      <c r="J12" s="76"/>
+      <c r="J12" s="75"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -3751,18 +3883,18 @@
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="57" t="s">
+      <c r="A13" s="54"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="56" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="21"/>
-      <c r="J13" s="76"/>
+      <c r="J13" s="75"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -3771,18 +3903,18 @@
       <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="57" t="s">
+      <c r="A14" s="54"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="56" t="s">
         <v>230</v>
       </c>
       <c r="I14" s="21"/>
-      <c r="J14" s="76"/>
+      <c r="J14" s="75"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -3791,38 +3923,38 @@
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="57" t="s">
+      <c r="A15" s="54"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="56" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="76"/>
+      <c r="J15" s="75"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
-      <c r="N15" s="30"/>
+      <c r="N15" s="29"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="57" t="s">
+      <c r="A16" s="54"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="56" t="s">
         <v>231</v>
       </c>
       <c r="I16" s="21"/>
-      <c r="J16" s="76"/>
+      <c r="J16" s="75"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="4"/>
@@ -3831,18 +3963,18 @@
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="58" t="s">
+      <c r="A17" s="59"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="78"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="77"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="4"/>
@@ -3851,18 +3983,18 @@
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
       <c r="G18" s="19"/>
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
-      <c r="J18" s="76"/>
+      <c r="J18" s="75"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="4"/>
@@ -3871,20 +4003,20 @@
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="60" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
       <c r="I19" s="20"/>
-      <c r="J19" s="31"/>
+      <c r="J19" s="30"/>
       <c r="L19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -3892,20 +4024,20 @@
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="78"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="77"/>
       <c r="L20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -3913,64 +4045,64 @@
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="56" t="s">
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
       <c r="G21" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="75"/>
+      <c r="H21" s="74"/>
       <c r="I21" s="21"/>
-      <c r="J21" s="76"/>
-      <c r="L21" s="35"/>
+      <c r="J21" s="75"/>
+      <c r="L21" s="34"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="63"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="56" t="s">
+      <c r="A22" s="62"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
       <c r="G22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="75"/>
+      <c r="H22" s="74"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="76"/>
+      <c r="J22" s="75"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="30"/>
+      <c r="N22" s="29"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="63"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="56" t="s">
+      <c r="A23" s="62"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
       <c r="G23" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="75"/>
+      <c r="H23" s="74"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="76"/>
+      <c r="J23" s="75"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="N23" s="4"/>
@@ -3979,20 +4111,20 @@
       <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="63"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="56" t="s">
+      <c r="A24" s="62"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
       <c r="G24" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="75"/>
+      <c r="H24" s="74"/>
       <c r="I24" s="21"/>
-      <c r="J24" s="76"/>
+      <c r="J24" s="75"/>
       <c r="L24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -4000,20 +4132,20 @@
       <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="63"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="56" t="s">
+      <c r="A25" s="62"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
       <c r="G25" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="75"/>
+      <c r="H25" s="74"/>
       <c r="I25" s="21"/>
-      <c r="J25" s="76"/>
+      <c r="J25" s="75"/>
       <c r="L25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -4021,20 +4153,20 @@
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="63"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="56" t="s">
+      <c r="A26" s="62"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
       <c r="G26" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="75"/>
+      <c r="H26" s="74"/>
       <c r="I26" s="21"/>
-      <c r="J26" s="76"/>
+      <c r="J26" s="75"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="N26" s="4"/>
@@ -4043,20 +4175,20 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="63"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="56" t="s">
+      <c r="A27" s="62"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
       <c r="G27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H27" s="75"/>
+      <c r="H27" s="74"/>
       <c r="I27" s="21"/>
-      <c r="J27" s="76"/>
+      <c r="J27" s="75"/>
       <c r="L27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -4064,20 +4196,18 @@
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="63"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="56" t="s">
+      <c r="A28" s="62"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" s="75"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="74"/>
       <c r="I28" s="21"/>
-      <c r="J28" s="76"/>
+      <c r="J28" s="75"/>
       <c r="L28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -4085,20 +4215,18 @@
       <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="63"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="56" t="s">
+      <c r="A29" s="62"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="95" t="s">
-        <v>254</v>
-      </c>
-      <c r="H29" s="75"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="74"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="76"/>
+      <c r="J29" s="75"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="18"/>
@@ -4108,18 +4236,18 @@
       <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="63"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="56" t="s">
+      <c r="A30" s="62"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="75"/>
+      <c r="H30" s="74"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="76"/>
+      <c r="J30" s="75"/>
       <c r="L30" s="4"/>
       <c r="M30" s="18"/>
       <c r="N30" s="4"/>
@@ -4128,18 +4256,18 @@
       <c r="Q30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="63"/>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="56" t="s">
+      <c r="A31" s="62"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="75"/>
+      <c r="H31" s="74"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="76"/>
+      <c r="J31" s="75"/>
       <c r="L31" s="4"/>
       <c r="M31" s="18"/>
       <c r="N31" s="4"/>
@@ -4148,18 +4276,18 @@
       <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="63"/>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="56" t="s">
+      <c r="A32" s="62"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="75"/>
+      <c r="H32" s="74"/>
       <c r="I32" s="21"/>
-      <c r="J32" s="76"/>
+      <c r="J32" s="75"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -4169,20 +4297,20 @@
       <c r="Q32" s="4"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="80"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="72"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="71"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="31"/>
+      <c r="J33" s="30"/>
       <c r="K33" s="13"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -4192,1217 +4320,1217 @@
       <c r="Q33" s="4"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="64" t="s">
+      <c r="A34" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
       <c r="I34" s="20"/>
-      <c r="J34" s="31"/>
+      <c r="J34" s="30"/>
       <c r="K34" s="13"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="60" t="s">
+      <c r="A35" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="77"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="78"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="77"/>
       <c r="K35" s="13"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="64" t="s">
+      <c r="A36" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="72"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="82" t="s">
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="F36" s="82" t="s">
+      <c r="F36" s="81" t="s">
         <v>234</v>
       </c>
-      <c r="G36" s="82" t="s">
+      <c r="G36" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="H36" s="45" t="s">
+      <c r="H36" s="44" t="s">
         <v>19</v>
       </c>
       <c r="I36" s="20"/>
-      <c r="J36" s="31"/>
+      <c r="J36" s="30"/>
       <c r="K36" s="13"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="60"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="81" t="s">
+      <c r="A37" s="59"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="I37" s="32"/>
-      <c r="J37" s="78"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="77"/>
       <c r="K37" s="13"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="65" t="s">
+      <c r="A38" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="71"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="70"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="55" t="s">
         <v>96</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="72"/>
-      <c r="H39" s="72"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
       <c r="I39" s="20"/>
-      <c r="J39" s="31"/>
+      <c r="J39" s="30"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="55" t="s">
         <v>97</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="75"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
       <c r="I40" s="21"/>
-      <c r="J40" s="76"/>
+      <c r="J40" s="75"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="56" t="s">
+      <c r="A41" s="55" t="s">
         <v>98</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
       <c r="I41" s="21"/>
-      <c r="J41" s="76"/>
+      <c r="J41" s="75"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="55" t="s">
         <v>99</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="75"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
       <c r="I42" s="21"/>
-      <c r="J42" s="76"/>
+      <c r="J42" s="75"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="55" t="s">
         <v>100</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="75"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="75"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
       <c r="I43" s="21"/>
-      <c r="J43" s="76"/>
+      <c r="J43" s="75"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="56" t="s">
+      <c r="A44" s="55" t="s">
         <v>101</v>
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="75"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="74"/>
       <c r="I44" s="21"/>
-      <c r="J44" s="76"/>
+      <c r="J44" s="75"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="55" t="s">
         <v>102</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="75"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="74"/>
       <c r="I45" s="21"/>
-      <c r="J45" s="76"/>
+      <c r="J45" s="75"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="55" t="s">
         <v>103</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="75"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
       <c r="I46" s="21"/>
-      <c r="J46" s="76"/>
+      <c r="J46" s="75"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="55" t="s">
         <v>104</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="74"/>
+      <c r="H47" s="74"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="76"/>
+      <c r="J47" s="75"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="56" t="s">
+      <c r="A48" s="55" t="s">
         <v>105</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="75"/>
-      <c r="H48" s="75"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="74"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="76"/>
+      <c r="J48" s="75"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="55" t="s">
         <v>106</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="75"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="74"/>
       <c r="I49" s="21"/>
-      <c r="J49" s="76"/>
+      <c r="J49" s="75"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="55" t="s">
         <v>107</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="75"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
       <c r="I50" s="21"/>
-      <c r="J50" s="76"/>
+      <c r="J50" s="75"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="55" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="75"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="74"/>
       <c r="I51" s="21"/>
-      <c r="J51" s="76"/>
+      <c r="J51" s="75"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="55" t="s">
         <v>109</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
+      <c r="H52" s="74"/>
       <c r="I52" s="21"/>
-      <c r="J52" s="76"/>
+      <c r="J52" s="75"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="56" t="s">
+      <c r="A53" s="55" t="s">
         <v>110</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="75"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="74"/>
+      <c r="H53" s="74"/>
       <c r="I53" s="21"/>
-      <c r="J53" s="76"/>
+      <c r="J53" s="75"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="56" t="s">
+      <c r="A54" s="55" t="s">
         <v>111</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="75"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="74"/>
+      <c r="H54" s="74"/>
       <c r="I54" s="21"/>
-      <c r="J54" s="76"/>
+      <c r="J54" s="75"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="65" t="s">
         <v>112</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="75"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="74"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="74"/>
+      <c r="H55" s="74"/>
       <c r="I55" s="21"/>
-      <c r="J55" s="76"/>
+      <c r="J55" s="75"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="65" t="s">
         <v>113</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="75"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="74"/>
+      <c r="H56" s="74"/>
       <c r="I56" s="21"/>
-      <c r="J56" s="76"/>
+      <c r="J56" s="75"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="65" t="s">
         <v>114</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="75"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="74"/>
+      <c r="F57" s="74"/>
+      <c r="G57" s="74"/>
+      <c r="H57" s="74"/>
       <c r="I57" s="21"/>
-      <c r="J57" s="76"/>
+      <c r="J57" s="75"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="65" t="s">
         <v>115</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
       <c r="I58" s="21"/>
-      <c r="J58" s="76"/>
+      <c r="J58" s="75"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="66" t="s">
+      <c r="A59" s="65" t="s">
         <v>116</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="75"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="75"/>
-      <c r="H59" s="75"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="74"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="74"/>
+      <c r="H59" s="74"/>
       <c r="I59" s="21"/>
-      <c r="J59" s="76"/>
+      <c r="J59" s="75"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="65" t="s">
         <v>117</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="75"/>
+      <c r="D60" s="74"/>
+      <c r="E60" s="74"/>
+      <c r="F60" s="74"/>
+      <c r="G60" s="74"/>
+      <c r="H60" s="74"/>
       <c r="I60" s="21"/>
-      <c r="J60" s="76"/>
+      <c r="J60" s="75"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="65" t="s">
         <v>118</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="21"/>
-      <c r="D61" s="75"/>
-      <c r="E61" s="75"/>
-      <c r="F61" s="75"/>
-      <c r="G61" s="75"/>
-      <c r="H61" s="75"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="74"/>
+      <c r="F61" s="74"/>
+      <c r="G61" s="74"/>
+      <c r="H61" s="74"/>
       <c r="I61" s="21"/>
-      <c r="J61" s="76"/>
+      <c r="J61" s="75"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="66" t="s">
+      <c r="A62" s="65" t="s">
         <v>119</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="75"/>
-      <c r="F62" s="75"/>
-      <c r="G62" s="75"/>
-      <c r="H62" s="75"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="74"/>
+      <c r="H62" s="74"/>
       <c r="I62" s="21"/>
-      <c r="J62" s="76"/>
+      <c r="J62" s="75"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="66" t="s">
+      <c r="A63" s="65" t="s">
         <v>120</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="74"/>
+      <c r="G63" s="74"/>
+      <c r="H63" s="74"/>
       <c r="I63" s="21"/>
-      <c r="J63" s="76"/>
+      <c r="J63" s="75"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="66" t="s">
+      <c r="A64" s="65" t="s">
         <v>121</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="75"/>
-      <c r="H64" s="75"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
+      <c r="F64" s="74"/>
+      <c r="G64" s="74"/>
+      <c r="H64" s="74"/>
       <c r="I64" s="21"/>
-      <c r="J64" s="76"/>
+      <c r="J64" s="75"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="66" t="s">
+      <c r="A65" s="65" t="s">
         <v>122</v>
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
+      <c r="F65" s="74"/>
+      <c r="G65" s="74"/>
+      <c r="H65" s="74"/>
       <c r="I65" s="21"/>
-      <c r="J65" s="76"/>
+      <c r="J65" s="75"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="66" t="s">
+      <c r="A66" s="65" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="21"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
       <c r="I66" s="21"/>
-      <c r="J66" s="76"/>
+      <c r="J66" s="75"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="66" t="s">
+      <c r="A67" s="65" t="s">
         <v>124</v>
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
+      <c r="F67" s="74"/>
+      <c r="G67" s="74"/>
+      <c r="H67" s="74"/>
       <c r="I67" s="21"/>
-      <c r="J67" s="76"/>
+      <c r="J67" s="75"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="66" t="s">
+      <c r="A68" s="65" t="s">
         <v>125</v>
       </c>
       <c r="B68" s="21"/>
       <c r="C68" s="21"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
+      <c r="F68" s="74"/>
+      <c r="G68" s="74"/>
+      <c r="H68" s="74"/>
       <c r="I68" s="21"/>
-      <c r="J68" s="76"/>
+      <c r="J68" s="75"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="66" t="s">
+      <c r="A69" s="65" t="s">
         <v>126</v>
       </c>
       <c r="B69" s="21"/>
       <c r="C69" s="21"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="75"/>
-      <c r="H69" s="75"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
+      <c r="F69" s="74"/>
+      <c r="G69" s="74"/>
+      <c r="H69" s="74"/>
       <c r="I69" s="21"/>
-      <c r="J69" s="76"/>
+      <c r="J69" s="75"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="66" t="s">
+      <c r="A70" s="65" t="s">
         <v>127</v>
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
-      <c r="D70" s="75"/>
-      <c r="E70" s="75"/>
-      <c r="F70" s="75"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
+      <c r="D70" s="74"/>
+      <c r="E70" s="74"/>
+      <c r="F70" s="74"/>
+      <c r="G70" s="74"/>
+      <c r="H70" s="74"/>
       <c r="I70" s="21"/>
-      <c r="J70" s="76"/>
+      <c r="J70" s="75"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="66" t="s">
+      <c r="A71" s="65" t="s">
         <v>128</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="21"/>
-      <c r="D71" s="75"/>
-      <c r="E71" s="75"/>
-      <c r="F71" s="75"/>
-      <c r="G71" s="75"/>
-      <c r="H71" s="75"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="74"/>
+      <c r="F71" s="74"/>
+      <c r="G71" s="74"/>
+      <c r="H71" s="74"/>
       <c r="I71" s="21"/>
-      <c r="J71" s="76"/>
+      <c r="J71" s="75"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="66" t="s">
+      <c r="A72" s="65" t="s">
         <v>129</v>
       </c>
       <c r="B72" s="21"/>
       <c r="C72" s="21"/>
-      <c r="D72" s="75"/>
-      <c r="E72" s="75"/>
-      <c r="F72" s="75"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
+      <c r="D72" s="74"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="74"/>
+      <c r="G72" s="74"/>
+      <c r="H72" s="74"/>
       <c r="I72" s="21"/>
-      <c r="J72" s="76"/>
+      <c r="J72" s="75"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="66" t="s">
+      <c r="A73" s="65" t="s">
         <v>130</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
+      <c r="D73" s="74"/>
+      <c r="E73" s="74"/>
+      <c r="F73" s="74"/>
+      <c r="G73" s="74"/>
+      <c r="H73" s="74"/>
       <c r="I73" s="21"/>
-      <c r="J73" s="76"/>
+      <c r="J73" s="75"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="66" t="s">
+      <c r="A74" s="65" t="s">
         <v>131</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
-      <c r="D74" s="75"/>
-      <c r="E74" s="75"/>
-      <c r="F74" s="75"/>
-      <c r="G74" s="75"/>
-      <c r="H74" s="75"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="74"/>
+      <c r="H74" s="74"/>
       <c r="I74" s="21"/>
-      <c r="J74" s="76"/>
+      <c r="J74" s="75"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="66" t="s">
+      <c r="A75" s="65" t="s">
         <v>132</v>
       </c>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="75"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="74"/>
+      <c r="G75" s="74"/>
+      <c r="H75" s="74"/>
       <c r="I75" s="21"/>
-      <c r="J75" s="76"/>
+      <c r="J75" s="75"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="66" t="s">
+      <c r="A76" s="65" t="s">
         <v>133</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
-      <c r="D76" s="75"/>
-      <c r="E76" s="75"/>
-      <c r="F76" s="75"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
+      <c r="D76" s="74"/>
+      <c r="E76" s="74"/>
+      <c r="F76" s="74"/>
+      <c r="G76" s="74"/>
+      <c r="H76" s="74"/>
       <c r="I76" s="21"/>
-      <c r="J76" s="76"/>
+      <c r="J76" s="75"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="66" t="s">
+      <c r="A77" s="65" t="s">
         <v>134</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="74"/>
+      <c r="G77" s="74"/>
+      <c r="H77" s="74"/>
       <c r="I77" s="21"/>
-      <c r="J77" s="76"/>
+      <c r="J77" s="75"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="66" t="s">
+      <c r="A78" s="65" t="s">
         <v>135</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
-      <c r="D78" s="75"/>
-      <c r="E78" s="75"/>
-      <c r="F78" s="75"/>
-      <c r="G78" s="75"/>
-      <c r="H78" s="75"/>
+      <c r="D78" s="74"/>
+      <c r="E78" s="74"/>
+      <c r="F78" s="74"/>
+      <c r="G78" s="74"/>
+      <c r="H78" s="74"/>
       <c r="I78" s="21"/>
-      <c r="J78" s="76"/>
+      <c r="J78" s="75"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="66" t="s">
+      <c r="A79" s="65" t="s">
         <v>136</v>
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
-      <c r="D79" s="75"/>
-      <c r="E79" s="75"/>
-      <c r="F79" s="75"/>
-      <c r="G79" s="75"/>
-      <c r="H79" s="75"/>
+      <c r="D79" s="74"/>
+      <c r="E79" s="74"/>
+      <c r="F79" s="74"/>
+      <c r="G79" s="74"/>
+      <c r="H79" s="74"/>
       <c r="I79" s="21"/>
-      <c r="J79" s="76"/>
+      <c r="J79" s="75"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="66" t="s">
+      <c r="A80" s="65" t="s">
         <v>137</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="21"/>
-      <c r="D80" s="75"/>
-      <c r="E80" s="75"/>
-      <c r="F80" s="75"/>
-      <c r="G80" s="75"/>
-      <c r="H80" s="75"/>
+      <c r="D80" s="74"/>
+      <c r="E80" s="74"/>
+      <c r="F80" s="74"/>
+      <c r="G80" s="74"/>
+      <c r="H80" s="74"/>
       <c r="I80" s="21"/>
-      <c r="J80" s="76"/>
+      <c r="J80" s="75"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="66" t="s">
+      <c r="A81" s="65" t="s">
         <v>138</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
+      <c r="F81" s="74"/>
+      <c r="G81" s="74"/>
+      <c r="H81" s="74"/>
       <c r="I81" s="21"/>
-      <c r="J81" s="76"/>
+      <c r="J81" s="75"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="66" t="s">
+      <c r="A82" s="65" t="s">
         <v>139</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="21"/>
-      <c r="D82" s="75"/>
-      <c r="E82" s="75"/>
-      <c r="F82" s="75"/>
-      <c r="G82" s="75"/>
-      <c r="H82" s="75"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+      <c r="F82" s="74"/>
+      <c r="G82" s="74"/>
+      <c r="H82" s="74"/>
       <c r="I82" s="21"/>
-      <c r="J82" s="76"/>
+      <c r="J82" s="75"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="66" t="s">
+      <c r="A83" s="65" t="s">
         <v>140</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="21"/>
-      <c r="D83" s="75"/>
-      <c r="E83" s="75"/>
-      <c r="F83" s="75"/>
-      <c r="G83" s="75"/>
-      <c r="H83" s="75"/>
+      <c r="D83" s="74"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="74"/>
+      <c r="G83" s="74"/>
+      <c r="H83" s="74"/>
       <c r="I83" s="21"/>
-      <c r="J83" s="76"/>
+      <c r="J83" s="75"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="66" t="s">
+      <c r="A84" s="65" t="s">
         <v>141</v>
       </c>
       <c r="B84" s="21"/>
       <c r="C84" s="21"/>
-      <c r="D84" s="75"/>
-      <c r="E84" s="75"/>
-      <c r="F84" s="75"/>
-      <c r="G84" s="75"/>
-      <c r="H84" s="75"/>
+      <c r="D84" s="74"/>
+      <c r="E84" s="74"/>
+      <c r="F84" s="74"/>
+      <c r="G84" s="74"/>
+      <c r="H84" s="74"/>
       <c r="I84" s="21"/>
-      <c r="J84" s="76"/>
+      <c r="J84" s="75"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="66" t="s">
+      <c r="A85" s="65" t="s">
         <v>142</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
-      <c r="D85" s="75"/>
-      <c r="E85" s="75"/>
-      <c r="F85" s="75"/>
-      <c r="G85" s="75"/>
-      <c r="H85" s="75"/>
+      <c r="D85" s="74"/>
+      <c r="E85" s="74"/>
+      <c r="F85" s="74"/>
+      <c r="G85" s="74"/>
+      <c r="H85" s="74"/>
       <c r="I85" s="21"/>
-      <c r="J85" s="76"/>
+      <c r="J85" s="75"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="66" t="s">
+      <c r="A86" s="65" t="s">
         <v>143</v>
       </c>
       <c r="B86" s="21"/>
       <c r="C86" s="21"/>
-      <c r="D86" s="75"/>
-      <c r="E86" s="75"/>
-      <c r="F86" s="75"/>
-      <c r="G86" s="75"/>
-      <c r="H86" s="75"/>
+      <c r="D86" s="74"/>
+      <c r="E86" s="74"/>
+      <c r="F86" s="74"/>
+      <c r="G86" s="74"/>
+      <c r="H86" s="74"/>
       <c r="I86" s="21"/>
-      <c r="J86" s="76"/>
+      <c r="J86" s="75"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="66" t="s">
+      <c r="A87" s="65" t="s">
         <v>144</v>
       </c>
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
-      <c r="D87" s="75"/>
-      <c r="E87" s="75"/>
-      <c r="F87" s="75"/>
-      <c r="G87" s="75"/>
-      <c r="H87" s="75"/>
+      <c r="D87" s="74"/>
+      <c r="E87" s="74"/>
+      <c r="F87" s="74"/>
+      <c r="G87" s="74"/>
+      <c r="H87" s="74"/>
       <c r="I87" s="21"/>
-      <c r="J87" s="76"/>
+      <c r="J87" s="75"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="66" t="s">
+      <c r="A88" s="65" t="s">
         <v>145</v>
       </c>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
-      <c r="D88" s="75"/>
-      <c r="E88" s="75"/>
-      <c r="F88" s="75"/>
-      <c r="G88" s="75"/>
-      <c r="H88" s="75"/>
+      <c r="D88" s="74"/>
+      <c r="E88" s="74"/>
+      <c r="F88" s="74"/>
+      <c r="G88" s="74"/>
+      <c r="H88" s="74"/>
       <c r="I88" s="21"/>
-      <c r="J88" s="76"/>
+      <c r="J88" s="75"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="66" t="s">
+      <c r="A89" s="65" t="s">
         <v>146</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
-      <c r="D89" s="75"/>
-      <c r="E89" s="75"/>
-      <c r="F89" s="75"/>
-      <c r="G89" s="75"/>
-      <c r="H89" s="75"/>
+      <c r="D89" s="74"/>
+      <c r="E89" s="74"/>
+      <c r="F89" s="74"/>
+      <c r="G89" s="74"/>
+      <c r="H89" s="74"/>
       <c r="I89" s="21"/>
-      <c r="J89" s="76"/>
+      <c r="J89" s="75"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="66" t="s">
+      <c r="A90" s="65" t="s">
         <v>147</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
-      <c r="D90" s="75"/>
-      <c r="E90" s="75"/>
-      <c r="F90" s="75"/>
-      <c r="G90" s="75"/>
-      <c r="H90" s="75"/>
+      <c r="D90" s="74"/>
+      <c r="E90" s="74"/>
+      <c r="F90" s="74"/>
+      <c r="G90" s="74"/>
+      <c r="H90" s="74"/>
       <c r="I90" s="21"/>
-      <c r="J90" s="76"/>
+      <c r="J90" s="75"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="66" t="s">
+      <c r="A91" s="65" t="s">
         <v>148</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
-      <c r="D91" s="75"/>
-      <c r="E91" s="75"/>
-      <c r="F91" s="75"/>
-      <c r="G91" s="75"/>
-      <c r="H91" s="75"/>
+      <c r="D91" s="74"/>
+      <c r="E91" s="74"/>
+      <c r="F91" s="74"/>
+      <c r="G91" s="74"/>
+      <c r="H91" s="74"/>
       <c r="I91" s="21"/>
-      <c r="J91" s="76"/>
+      <c r="J91" s="75"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="66" t="s">
+      <c r="A92" s="65" t="s">
         <v>149</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="21"/>
-      <c r="D92" s="75"/>
-      <c r="E92" s="75"/>
-      <c r="F92" s="75"/>
-      <c r="G92" s="75"/>
-      <c r="H92" s="75"/>
+      <c r="D92" s="74"/>
+      <c r="E92" s="74"/>
+      <c r="F92" s="74"/>
+      <c r="G92" s="74"/>
+      <c r="H92" s="74"/>
       <c r="I92" s="21"/>
-      <c r="J92" s="76"/>
+      <c r="J92" s="75"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="66" t="s">
+      <c r="A93" s="65" t="s">
         <v>150</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="21"/>
-      <c r="D93" s="75"/>
-      <c r="E93" s="75"/>
-      <c r="F93" s="75"/>
-      <c r="G93" s="75"/>
-      <c r="H93" s="75"/>
+      <c r="D93" s="74"/>
+      <c r="E93" s="74"/>
+      <c r="F93" s="74"/>
+      <c r="G93" s="74"/>
+      <c r="H93" s="74"/>
       <c r="I93" s="21"/>
-      <c r="J93" s="76"/>
+      <c r="J93" s="75"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="66" t="s">
+      <c r="A94" s="65" t="s">
         <v>151</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
-      <c r="D94" s="75"/>
-      <c r="E94" s="75"/>
-      <c r="F94" s="75"/>
-      <c r="G94" s="75"/>
-      <c r="H94" s="75"/>
+      <c r="D94" s="74"/>
+      <c r="E94" s="74"/>
+      <c r="F94" s="74"/>
+      <c r="G94" s="74"/>
+      <c r="H94" s="74"/>
       <c r="I94" s="21"/>
-      <c r="J94" s="76"/>
+      <c r="J94" s="75"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="66" t="s">
+      <c r="A95" s="65" t="s">
         <v>152</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="21"/>
-      <c r="D95" s="75"/>
-      <c r="E95" s="75"/>
-      <c r="F95" s="75"/>
-      <c r="G95" s="75"/>
-      <c r="H95" s="75"/>
+      <c r="D95" s="74"/>
+      <c r="E95" s="74"/>
+      <c r="F95" s="74"/>
+      <c r="G95" s="74"/>
+      <c r="H95" s="74"/>
       <c r="I95" s="21"/>
-      <c r="J95" s="76"/>
+      <c r="J95" s="75"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="66" t="s">
+      <c r="A96" s="65" t="s">
         <v>153</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="21"/>
-      <c r="D96" s="75"/>
-      <c r="E96" s="75"/>
-      <c r="F96" s="75"/>
-      <c r="G96" s="75"/>
-      <c r="H96" s="75"/>
+      <c r="D96" s="74"/>
+      <c r="E96" s="74"/>
+      <c r="F96" s="74"/>
+      <c r="G96" s="74"/>
+      <c r="H96" s="74"/>
       <c r="I96" s="21"/>
-      <c r="J96" s="76"/>
+      <c r="J96" s="75"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="66" t="s">
+      <c r="A97" s="65" t="s">
         <v>154</v>
       </c>
       <c r="B97" s="21"/>
       <c r="C97" s="21"/>
-      <c r="D97" s="75"/>
-      <c r="E97" s="75"/>
-      <c r="F97" s="75"/>
-      <c r="G97" s="75"/>
-      <c r="H97" s="75"/>
+      <c r="D97" s="74"/>
+      <c r="E97" s="74"/>
+      <c r="F97" s="74"/>
+      <c r="G97" s="74"/>
+      <c r="H97" s="74"/>
       <c r="I97" s="21"/>
-      <c r="J97" s="76"/>
+      <c r="J97" s="75"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="66" t="s">
+      <c r="A98" s="65" t="s">
         <v>155</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="21"/>
-      <c r="D98" s="75"/>
-      <c r="E98" s="75"/>
-      <c r="F98" s="75"/>
-      <c r="G98" s="75"/>
-      <c r="H98" s="75"/>
+      <c r="D98" s="74"/>
+      <c r="E98" s="74"/>
+      <c r="F98" s="74"/>
+      <c r="G98" s="74"/>
+      <c r="H98" s="74"/>
       <c r="I98" s="21"/>
-      <c r="J98" s="76"/>
+      <c r="J98" s="75"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="66" t="s">
+      <c r="A99" s="65" t="s">
         <v>156</v>
       </c>
       <c r="B99" s="21"/>
       <c r="C99" s="21"/>
-      <c r="D99" s="75"/>
-      <c r="E99" s="75"/>
-      <c r="F99" s="75"/>
-      <c r="G99" s="75"/>
-      <c r="H99" s="75"/>
+      <c r="D99" s="74"/>
+      <c r="E99" s="74"/>
+      <c r="F99" s="74"/>
+      <c r="G99" s="74"/>
+      <c r="H99" s="74"/>
       <c r="I99" s="21"/>
-      <c r="J99" s="76"/>
+      <c r="J99" s="75"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="66" t="s">
+      <c r="A100" s="65" t="s">
         <v>157</v>
       </c>
       <c r="B100" s="21"/>
       <c r="C100" s="21"/>
-      <c r="D100" s="75"/>
-      <c r="E100" s="75"/>
-      <c r="F100" s="75"/>
-      <c r="G100" s="75"/>
-      <c r="H100" s="75"/>
+      <c r="D100" s="74"/>
+      <c r="E100" s="74"/>
+      <c r="F100" s="74"/>
+      <c r="G100" s="74"/>
+      <c r="H100" s="74"/>
       <c r="I100" s="21"/>
-      <c r="J100" s="76"/>
+      <c r="J100" s="75"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="66" t="s">
+      <c r="A101" s="65" t="s">
         <v>158</v>
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="21"/>
-      <c r="D101" s="75"/>
-      <c r="E101" s="75"/>
-      <c r="F101" s="75"/>
-      <c r="G101" s="75"/>
-      <c r="H101" s="75"/>
+      <c r="D101" s="74"/>
+      <c r="E101" s="74"/>
+      <c r="F101" s="74"/>
+      <c r="G101" s="74"/>
+      <c r="H101" s="74"/>
       <c r="I101" s="21"/>
-      <c r="J101" s="76"/>
+      <c r="J101" s="75"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="66" t="s">
+      <c r="A102" s="65" t="s">
         <v>159</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="21"/>
-      <c r="D102" s="75"/>
-      <c r="E102" s="75"/>
-      <c r="F102" s="75"/>
-      <c r="G102" s="75"/>
-      <c r="H102" s="75"/>
+      <c r="D102" s="74"/>
+      <c r="E102" s="74"/>
+      <c r="F102" s="74"/>
+      <c r="G102" s="74"/>
+      <c r="H102" s="74"/>
       <c r="I102" s="21"/>
-      <c r="J102" s="76"/>
+      <c r="J102" s="75"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="66" t="s">
+      <c r="A103" s="65" t="s">
         <v>160</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="21"/>
-      <c r="D103" s="75"/>
-      <c r="E103" s="75"/>
-      <c r="F103" s="75"/>
-      <c r="G103" s="75"/>
-      <c r="H103" s="75"/>
+      <c r="D103" s="74"/>
+      <c r="E103" s="74"/>
+      <c r="F103" s="74"/>
+      <c r="G103" s="74"/>
+      <c r="H103" s="74"/>
       <c r="I103" s="21"/>
-      <c r="J103" s="76"/>
+      <c r="J103" s="75"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="66" t="s">
+      <c r="A104" s="65" t="s">
         <v>161</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="21"/>
-      <c r="D104" s="75"/>
-      <c r="E104" s="75"/>
-      <c r="F104" s="75"/>
-      <c r="G104" s="75"/>
-      <c r="H104" s="75"/>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="74"/>
+      <c r="G104" s="74"/>
+      <c r="H104" s="74"/>
       <c r="I104" s="21"/>
-      <c r="J104" s="76"/>
+      <c r="J104" s="75"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="66" t="s">
+      <c r="A105" s="65" t="s">
         <v>162</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="21"/>
-      <c r="D105" s="75"/>
-      <c r="E105" s="75"/>
-      <c r="F105" s="75"/>
-      <c r="G105" s="75"/>
-      <c r="H105" s="75"/>
+      <c r="D105" s="74"/>
+      <c r="E105" s="74"/>
+      <c r="F105" s="74"/>
+      <c r="G105" s="74"/>
+      <c r="H105" s="74"/>
       <c r="I105" s="21"/>
-      <c r="J105" s="76"/>
+      <c r="J105" s="75"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="66" t="s">
+      <c r="A106" s="65" t="s">
         <v>163</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="21"/>
-      <c r="D106" s="75"/>
-      <c r="E106" s="75"/>
-      <c r="F106" s="75"/>
-      <c r="G106" s="75"/>
-      <c r="H106" s="75"/>
+      <c r="D106" s="74"/>
+      <c r="E106" s="74"/>
+      <c r="F106" s="74"/>
+      <c r="G106" s="74"/>
+      <c r="H106" s="74"/>
       <c r="I106" s="21"/>
-      <c r="J106" s="76"/>
+      <c r="J106" s="75"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="66" t="s">
+      <c r="A107" s="65" t="s">
         <v>164</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="21"/>
-      <c r="D107" s="75"/>
-      <c r="E107" s="75"/>
-      <c r="F107" s="75"/>
-      <c r="G107" s="75"/>
-      <c r="H107" s="75"/>
+      <c r="D107" s="74"/>
+      <c r="E107" s="74"/>
+      <c r="F107" s="74"/>
+      <c r="G107" s="74"/>
+      <c r="H107" s="74"/>
       <c r="I107" s="21"/>
-      <c r="J107" s="76"/>
+      <c r="J107" s="75"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="66" t="s">
+      <c r="A108" s="65" t="s">
         <v>165</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="21"/>
-      <c r="D108" s="75"/>
-      <c r="E108" s="75"/>
-      <c r="F108" s="75"/>
-      <c r="G108" s="75"/>
-      <c r="H108" s="75"/>
+      <c r="D108" s="74"/>
+      <c r="E108" s="74"/>
+      <c r="F108" s="74"/>
+      <c r="G108" s="74"/>
+      <c r="H108" s="74"/>
       <c r="I108" s="21"/>
-      <c r="J108" s="76"/>
+      <c r="J108" s="75"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="66" t="s">
+      <c r="A109" s="65" t="s">
         <v>166</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="21"/>
-      <c r="D109" s="75"/>
-      <c r="E109" s="75"/>
-      <c r="F109" s="75"/>
-      <c r="G109" s="75"/>
-      <c r="H109" s="75"/>
+      <c r="D109" s="74"/>
+      <c r="E109" s="74"/>
+      <c r="F109" s="74"/>
+      <c r="G109" s="74"/>
+      <c r="H109" s="74"/>
       <c r="I109" s="21"/>
-      <c r="J109" s="76"/>
+      <c r="J109" s="75"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="66" t="s">
+      <c r="A110" s="65" t="s">
         <v>167</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="21"/>
-      <c r="D110" s="75"/>
-      <c r="E110" s="75"/>
-      <c r="F110" s="75"/>
-      <c r="G110" s="75"/>
-      <c r="H110" s="75"/>
+      <c r="D110" s="74"/>
+      <c r="E110" s="74"/>
+      <c r="F110" s="74"/>
+      <c r="G110" s="74"/>
+      <c r="H110" s="74"/>
       <c r="I110" s="21"/>
-      <c r="J110" s="76"/>
+      <c r="J110" s="75"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="66" t="s">
+      <c r="A111" s="65" t="s">
         <v>168</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="21"/>
-      <c r="D111" s="75"/>
-      <c r="E111" s="75"/>
-      <c r="F111" s="75"/>
-      <c r="G111" s="75"/>
-      <c r="H111" s="75"/>
+      <c r="D111" s="74"/>
+      <c r="E111" s="74"/>
+      <c r="F111" s="74"/>
+      <c r="G111" s="74"/>
+      <c r="H111" s="74"/>
       <c r="I111" s="21"/>
-      <c r="J111" s="76"/>
+      <c r="J111" s="75"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="66" t="s">
+      <c r="A112" s="65" t="s">
         <v>169</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="21"/>
-      <c r="D112" s="75"/>
-      <c r="E112" s="75"/>
-      <c r="F112" s="75"/>
-      <c r="G112" s="75"/>
-      <c r="H112" s="75"/>
+      <c r="D112" s="74"/>
+      <c r="E112" s="74"/>
+      <c r="F112" s="74"/>
+      <c r="G112" s="74"/>
+      <c r="H112" s="74"/>
       <c r="I112" s="21"/>
-      <c r="J112" s="76"/>
+      <c r="J112" s="75"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="66" t="s">
+      <c r="A113" s="65" t="s">
         <v>170</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="21"/>
-      <c r="D113" s="75"/>
-      <c r="E113" s="75"/>
-      <c r="F113" s="75"/>
-      <c r="G113" s="75"/>
-      <c r="H113" s="75"/>
+      <c r="D113" s="74"/>
+      <c r="E113" s="74"/>
+      <c r="F113" s="74"/>
+      <c r="G113" s="74"/>
+      <c r="H113" s="74"/>
       <c r="I113" s="21"/>
-      <c r="J113" s="76"/>
+      <c r="J113" s="75"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="66" t="s">
+      <c r="A114" s="65" t="s">
         <v>171</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="21"/>
-      <c r="D114" s="75"/>
-      <c r="E114" s="75"/>
-      <c r="F114" s="75"/>
-      <c r="G114" s="75"/>
-      <c r="H114" s="75"/>
+      <c r="D114" s="74"/>
+      <c r="E114" s="74"/>
+      <c r="F114" s="74"/>
+      <c r="G114" s="74"/>
+      <c r="H114" s="74"/>
       <c r="I114" s="21"/>
-      <c r="J114" s="76"/>
+      <c r="J114" s="75"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="66" t="s">
+      <c r="A115" s="65" t="s">
         <v>172</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="21"/>
-      <c r="D115" s="75"/>
-      <c r="E115" s="75"/>
-      <c r="F115" s="75"/>
-      <c r="G115" s="75"/>
-      <c r="H115" s="75"/>
+      <c r="D115" s="74"/>
+      <c r="E115" s="74"/>
+      <c r="F115" s="74"/>
+      <c r="G115" s="74"/>
+      <c r="H115" s="74"/>
       <c r="I115" s="21"/>
-      <c r="J115" s="76"/>
+      <c r="J115" s="75"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="66" t="s">
+      <c r="A116" s="65" t="s">
         <v>173</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="21"/>
-      <c r="D116" s="75"/>
-      <c r="E116" s="75"/>
-      <c r="F116" s="75"/>
-      <c r="G116" s="75"/>
-      <c r="H116" s="75"/>
+      <c r="D116" s="74"/>
+      <c r="E116" s="74"/>
+      <c r="F116" s="74"/>
+      <c r="G116" s="74"/>
+      <c r="H116" s="74"/>
       <c r="I116" s="21"/>
-      <c r="J116" s="76"/>
+      <c r="J116" s="75"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="66" t="s">
+      <c r="A117" s="65" t="s">
         <v>174</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="21"/>
-      <c r="D117" s="75"/>
-      <c r="E117" s="75"/>
-      <c r="F117" s="75"/>
-      <c r="G117" s="75"/>
-      <c r="H117" s="75"/>
+      <c r="D117" s="74"/>
+      <c r="E117" s="74"/>
+      <c r="F117" s="74"/>
+      <c r="G117" s="74"/>
+      <c r="H117" s="74"/>
       <c r="I117" s="21"/>
-      <c r="J117" s="76"/>
+      <c r="J117" s="75"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="67" t="s">
+      <c r="A118" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="B118" s="32"/>
-      <c r="C118" s="32"/>
-      <c r="D118" s="77"/>
-      <c r="E118" s="77"/>
-      <c r="F118" s="77"/>
-      <c r="G118" s="77"/>
-      <c r="H118" s="77"/>
-      <c r="I118" s="32"/>
-      <c r="J118" s="78"/>
+      <c r="B118" s="31"/>
+      <c r="C118" s="31"/>
+      <c r="D118" s="76"/>
+      <c r="E118" s="76"/>
+      <c r="F118" s="76"/>
+      <c r="G118" s="76"/>
+      <c r="H118" s="76"/>
+      <c r="I118" s="31"/>
+      <c r="J118" s="77"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F2">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>IF(OR(A2="",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>IF(OR(A2="_ascii",A2="_cmd",A2="_dektec"),0,1)</formula>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>IF(OR(A2="_ascii",A2="_HEX",A2="_cmd",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5410,25 +5538,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{C2964006-1830-40A2-88E7-53F888A2750B}">
-            <xm:f>IF(OR(Schedule!A2="_ascii",Schedule!A2="_cmd",Schedule!A2="_dektec"),0,1)</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="0" tint="-0.499984740745262"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H2</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5447,117 +5556,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="97"/>
+      <c r="B1" s="95"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-    </row>
-    <row r="4" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-    </row>
-    <row r="5" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+    </row>
+    <row r="5" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="38" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="40" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-    </row>
-    <row r="10" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+    </row>
+    <row r="10" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-    </row>
-    <row r="11" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+    </row>
+    <row r="11" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
1. Update version to v1.0.11. 2. Open the TX_board control item. 3. Fixed can't save the Canbus log issue. 4. Update Woodpecker_Script Template(With RC) V1.0.0_20191218 & Woodpecker_Script Template(Without RC) V1.0.0_20191224 version.
</commit_message>
<xml_diff>
--- a/branches/Woodpecker_All/Woodpecker/Woodpecker/Reference/Schedule/Woodpecker_Script Template(With RC).xlsx
+++ b/branches/Woodpecker_All/Woodpecker/Woodpecker/Reference/Schedule/Woodpecker_Script Template(With RC).xlsx
@@ -25,7 +25,7 @@
     <definedName name="_Pin">List!$D$11:$D$22</definedName>
     <definedName name="Cmd_list">List!$A$2:$A$96</definedName>
     <definedName name="COM">List!$D$2:$D$8</definedName>
-    <definedName name="CRC">List!$L$2:$L$3</definedName>
+    <definedName name="CRC">List!$E$2:$E$3</definedName>
     <definedName name="switch">List!$H$8:$H$17</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="256">
   <si>
     <t>SerialPort I/O comd</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1237,8 +1237,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>CRC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>CRC16_Modbus</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1690,6 +1693,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1881,49 +1887,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <fill>
         <patternFill>
@@ -1991,48 +1959,6 @@
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2395,16 +2321,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="87" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="88" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="89" t="s">
         <v>241</v>
       </c>
       <c r="E1" s="15" t="s">
@@ -2419,16 +2345,16 @@
       <c r="H1" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="90" t="s">
         <v>244</v>
       </c>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="91" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
-      <c r="B2" s="45"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -2440,7 +2366,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
-      <c r="B3" s="45"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -2452,7 +2378,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
-      <c r="B4" s="45"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -2464,7 +2390,7 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
-      <c r="B5" s="45"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -2476,7 +2402,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
-      <c r="B6" s="45"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -2488,7 +2414,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
-      <c r="B7" s="45"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -2500,7 +2426,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="45"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -2512,7 +2438,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
-      <c r="B9" s="45"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -2524,7 +2450,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
-      <c r="B10" s="45"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -2536,7 +2462,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
-      <c r="B11" s="45"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -2548,7 +2474,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
-      <c r="B12" s="45"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -2560,7 +2486,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
-      <c r="B13" s="45"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -2572,7 +2498,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="45"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -2584,7 +2510,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
-      <c r="B15" s="45"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -2596,7 +2522,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
-      <c r="B16" s="45"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -2608,7 +2534,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
-      <c r="B17" s="45"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2620,7 +2546,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
-      <c r="B18" s="45"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -2632,7 +2558,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
-      <c r="B19" s="45"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -2644,7 +2570,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
-      <c r="B20" s="45"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -2656,7 +2582,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
-      <c r="B21" s="45"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -2668,7 +2594,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
-      <c r="B22" s="45"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -2680,7 +2606,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
-      <c r="B23" s="45"/>
+      <c r="B23" s="46"/>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -2692,7 +2618,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
-      <c r="B24" s="45"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -2704,7 +2630,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
-      <c r="B25" s="45"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
@@ -2716,7 +2642,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
-      <c r="B26" s="45"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="23"/>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
@@ -2728,7 +2654,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
-      <c r="B27" s="45"/>
+      <c r="B27" s="46"/>
       <c r="C27" s="23"/>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
@@ -2740,7 +2666,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
-      <c r="B28" s="45"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="23"/>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
@@ -2752,7 +2678,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
-      <c r="B29" s="45"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="23"/>
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
@@ -2764,7 +2690,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
-      <c r="B30" s="45"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
@@ -2776,7 +2702,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
-      <c r="B31" s="45"/>
+      <c r="B31" s="46"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
@@ -2790,42 +2716,42 @@
   <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B31">
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="15" priority="8">
       <formula>IF(OR(A2="_HEX",A2="_ascii",A2="_shot",A2="_rc_start",A2="_rc_stop",A2="_cmd",A2="_DOS",A2="_Pin",A2="_quantum",A2="_astro",A2="_dektec"),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C31">
-    <cfRule type="expression" dxfId="19" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>IF(OR(A2="_HEX",A2="_ascii",A2="_shot",A2="_rc_start",A2="_rc_stop",A2="_cmd",A2="_DOS",A2="_IO_Output",A2="_IO_Input",A2="_Pin",A2="_keyword",A2="_quantum",A2="_astro",A2="_dektec"),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D31">
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>IF(OR(A2="",A2="_HEX",A2="_ascii",A2="_Pin"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E31">
-    <cfRule type="expression" dxfId="17" priority="5">
-      <formula>IF(OR(A2="",A2="_astro",A2="_quantum",A2="_dektec"),0,1)</formula>
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>IF(OR(A2="",A2="_HEX",A2="_astro",A2="_quantum",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>IF(OR(A2="",A2="_quantum",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>IF(OR(A2="",A2="_HEX",A2="_ascii",A2="_DOS",A2="_Pin",A2="_keyword",A2="_dektec",A2="_audio_debounce"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="expression" dxfId="13" priority="2">
-      <formula>IF(OR(A2="",A2="_ascii",A2="_HEX",A2="_cmd",A2="_dektec"),0,1)</formula>
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>IF(OR(A2="",A2="_ascii",A2="_cmd",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>IF(OR(G2="_save",G2="_clear"),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2837,14 +2763,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G31">
       <formula1>IF(OR(A2="_HEX",A2="_ascii"),_log,IF(E2="Front tyre",_ABS_front,IF(E2="Rare tyre",_ABS_rare,IF(E2="Other",_ABS_other,IF(A2="_Temperature",_temp,IF(OR(A2="_Pin",A2="_keyword"),_P_cmd,""))))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H31">
-      <formula1>IF(A3="_ascii",_NEL,IF(A3="_FuncKey",_NEL,IF(A3="_cmd",switch,IF(A3="_dektec",_dektec,""))))</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H31">
+      <formula1>IF(A2="_ascii",_NEL,IF(A2="_FuncKey",_NEL,IF(A2="_cmd",switch,IF(A2="_dektec",_dektec,""))))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31">
       <formula1>IF(OR(A2="_HEX",A2="_ascii",A2="_FuncKey"),COM,IF(A2="_Pin",_Pin,""))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
-      <formula1>IF(A2="_ascii",_NEL,IF(A2="_FuncKey",_NEL,IF(A2="_cmd",switch,IF(A2="_dektec",_dektec,IF(A2="_HEX",CRC,"")))))</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+      <formula1>IF(A2="_HEX",CRC,"")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2858,7 +2784,7 @@
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2880,7 +2806,7 @@
       <c r="C1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="93" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="16" t="s">
@@ -2909,13 +2835,14 @@
       <c r="D2" s="24" t="s">
         <v>36</v>
       </c>
+      <c r="E2" s="24" t="s">
+        <v>255</v>
+      </c>
       <c r="G2" s="24" t="s">
         <v>47</v>
       </c>
       <c r="K2" s="21"/>
-      <c r="L2" s="24" t="s">
-        <v>254</v>
-      </c>
+      <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2924,17 +2851,18 @@
       <c r="D3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="E3" s="26"/>
+      <c r="G3" s="92" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>42</v>
       </c>
       <c r="K3" s="21"/>
-      <c r="L3" s="26"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="25" t="s">
@@ -2971,7 +2899,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>177</v>
       </c>
       <c r="D7" s="25" t="s">
@@ -2979,23 +2907,23 @@
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="49" t="s">
         <v>178</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="H8" s="82" t="s">
+      <c r="H8" s="83" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="33" t="s">
         <v>179</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
-      <c r="H9" s="83" t="s">
+      <c r="H9" s="84" t="s">
         <v>3</v>
       </c>
       <c r="K9" s="24">
@@ -3003,12 +2931,12 @@
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="47" t="s">
         <v>180</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
-      <c r="H10" s="83" t="s">
+      <c r="H10" s="84" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="25">
@@ -3016,17 +2944,17 @@
       </c>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="50" t="s">
         <v>181</v>
       </c>
       <c r="C11" s="21"/>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="83" t="s">
+      <c r="H11" s="84" t="s">
         <v>6</v>
       </c>
       <c r="K11" s="25">
@@ -3039,13 +2967,13 @@
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="83" t="s">
+      <c r="H12" s="84" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="25">
@@ -3053,20 +2981,20 @@
       </c>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>183</v>
       </c>
       <c r="B13" s="24">
         <v>1</v>
       </c>
       <c r="C13" s="21"/>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="83" t="s">
+      <c r="H13" s="84" t="s">
         <v>7</v>
       </c>
       <c r="K13" s="25">
@@ -3081,14 +3009,14 @@
         <v>2</v>
       </c>
       <c r="C14" s="21"/>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="43" t="s">
         <v>56</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="83" t="s">
+      <c r="H14" s="84" t="s">
         <v>236</v>
       </c>
       <c r="K14" s="25">
@@ -3103,14 +3031,14 @@
         <v>3</v>
       </c>
       <c r="C15" s="21"/>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="43" t="s">
         <v>57</v>
       </c>
       <c r="E15" s="21"/>
       <c r="G15" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="83" t="s">
+      <c r="H15" s="84" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="25">
@@ -3125,14 +3053,14 @@
         <v>4</v>
       </c>
       <c r="C16" s="21"/>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="43" t="s">
         <v>58</v>
       </c>
       <c r="E16" s="21"/>
       <c r="G16" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="83" t="s">
+      <c r="H16" s="84" t="s">
         <v>235</v>
       </c>
       <c r="K16" s="25">
@@ -3147,14 +3075,14 @@
         <v>5</v>
       </c>
       <c r="C17" s="21"/>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="43" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="21"/>
       <c r="G17" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="84" t="s">
+      <c r="H17" s="85" t="s">
         <v>8</v>
       </c>
       <c r="K17" s="25">
@@ -3169,7 +3097,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="21"/>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="43" t="s">
         <v>60</v>
       </c>
       <c r="E18" s="21"/>
@@ -3188,11 +3116,11 @@
         <v>7</v>
       </c>
       <c r="C19" s="21"/>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="43" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="21"/>
-      <c r="H19" s="31"/>
+      <c r="H19" s="32"/>
       <c r="K19" s="25">
         <v>30</v>
       </c>
@@ -3204,11 +3132,11 @@
       <c r="B20" s="25">
         <v>8</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="43" t="s">
         <v>62</v>
       </c>
       <c r="E20" s="21"/>
-      <c r="H20" s="50" t="s">
+      <c r="H20" s="51" t="s">
         <v>90</v>
       </c>
       <c r="K20" s="25">
@@ -3222,7 +3150,7 @@
       <c r="B21" s="25">
         <v>9</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="43" t="s">
         <v>63</v>
       </c>
       <c r="H21" s="28" t="s">
@@ -3239,7 +3167,7 @@
       <c r="B22" s="26">
         <v>10</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="44" t="s">
         <v>64</v>
       </c>
       <c r="K22" s="25">
@@ -3647,7 +3575,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3709,172 +3637,172 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68" t="s">
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="69" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="96" t="s">
+      <c r="E2" s="48" t="s">
         <v>254</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="70"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="69" t="s">
         <v>233</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="33" t="s">
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="I3" s="69"/>
-      <c r="J3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="71"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="68" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="69" t="s">
         <v>233</v>
       </c>
-      <c r="E4" s="71"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="73" t="s">
+      <c r="E4" s="72"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="74" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="20"/>
-      <c r="J4" s="30"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="30"/>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="55" t="s">
         <v>247</v>
       </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
       <c r="I6" s="21"/>
-      <c r="J6" s="75"/>
+      <c r="J6" s="76"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="60" t="s">
         <v>248</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="77"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="78"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="56" t="s">
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="57" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="21"/>
-      <c r="J8" s="75"/>
+      <c r="J8" s="76"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="56" t="s">
+      <c r="A9" s="55"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="57" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="21"/>
-      <c r="J9" s="75"/>
+      <c r="J9" s="76"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="56" t="s">
+      <c r="A10" s="55"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="57" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="21"/>
-      <c r="J10" s="75"/>
+      <c r="J10" s="76"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="56" t="s">
+      <c r="A11" s="55"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="57" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="21"/>
-      <c r="J11" s="75"/>
+      <c r="J11" s="76"/>
     </row>
     <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="56" t="s">
+      <c r="A12" s="55"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="57" t="s">
         <v>10</v>
       </c>
       <c r="I12" s="21"/>
-      <c r="J12" s="75"/>
+      <c r="J12" s="76"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -3883,18 +3811,18 @@
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="56" t="s">
+      <c r="A13" s="55"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="57" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="21"/>
-      <c r="J13" s="75"/>
+      <c r="J13" s="76"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -3903,18 +3831,18 @@
       <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="56" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="57" t="s">
         <v>230</v>
       </c>
       <c r="I14" s="21"/>
-      <c r="J14" s="75"/>
+      <c r="J14" s="76"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -3923,38 +3851,38 @@
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="56" t="s">
+      <c r="A15" s="55"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="57" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="75"/>
+      <c r="J15" s="76"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
-      <c r="N15" s="29"/>
+      <c r="N15" s="30"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="56" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="57" t="s">
         <v>231</v>
       </c>
       <c r="I16" s="21"/>
-      <c r="J16" s="75"/>
+      <c r="J16" s="76"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="4"/>
@@ -3963,18 +3891,18 @@
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="57" t="s">
+      <c r="A17" s="60"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="77"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="78"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="4"/>
@@ -3983,18 +3911,18 @@
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
       <c r="G18" s="19"/>
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
-      <c r="J18" s="75"/>
+      <c r="J18" s="76"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="4"/>
@@ -4003,20 +3931,20 @@
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="61" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
       <c r="I19" s="20"/>
-      <c r="J19" s="30"/>
+      <c r="J19" s="31"/>
       <c r="L19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -4024,20 +3952,20 @@
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="78"/>
       <c r="L20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -4045,64 +3973,64 @@
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="55" t="s">
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
       <c r="G21" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="74"/>
+      <c r="H21" s="75"/>
       <c r="I21" s="21"/>
-      <c r="J21" s="75"/>
-      <c r="L21" s="34"/>
+      <c r="J21" s="76"/>
+      <c r="L21" s="35"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="55" t="s">
+      <c r="A22" s="63"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
       <c r="G22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="74"/>
+      <c r="H22" s="75"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="75"/>
+      <c r="J22" s="76"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="29"/>
+      <c r="N22" s="30"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="55" t="s">
+      <c r="A23" s="63"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
       <c r="G23" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="74"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="75"/>
+      <c r="J23" s="76"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="N23" s="4"/>
@@ -4111,20 +4039,20 @@
       <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="55" t="s">
+      <c r="A24" s="63"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
       <c r="G24" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="74"/>
+      <c r="H24" s="75"/>
       <c r="I24" s="21"/>
-      <c r="J24" s="75"/>
+      <c r="J24" s="76"/>
       <c r="L24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -4132,20 +4060,20 @@
       <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="55" t="s">
+      <c r="A25" s="63"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
       <c r="G25" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="74"/>
+      <c r="H25" s="75"/>
       <c r="I25" s="21"/>
-      <c r="J25" s="75"/>
+      <c r="J25" s="76"/>
       <c r="L25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -4153,20 +4081,20 @@
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="55" t="s">
+      <c r="A26" s="63"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
       <c r="G26" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="74"/>
+      <c r="H26" s="75"/>
       <c r="I26" s="21"/>
-      <c r="J26" s="75"/>
+      <c r="J26" s="76"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="N26" s="4"/>
@@ -4175,20 +4103,20 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="55" t="s">
+      <c r="A27" s="63"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
       <c r="G27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H27" s="74"/>
+      <c r="H27" s="75"/>
       <c r="I27" s="21"/>
-      <c r="J27" s="75"/>
+      <c r="J27" s="76"/>
       <c r="L27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -4196,18 +4124,18 @@
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="55" t="s">
+      <c r="A28" s="63"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
       <c r="G28" s="19"/>
-      <c r="H28" s="74"/>
+      <c r="H28" s="75"/>
       <c r="I28" s="21"/>
-      <c r="J28" s="75"/>
+      <c r="J28" s="76"/>
       <c r="L28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -4215,18 +4143,18 @@
       <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="55" t="s">
+      <c r="A29" s="63"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="74"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="75"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="75"/>
+      <c r="J29" s="76"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="18"/>
@@ -4236,18 +4164,18 @@
       <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="55" t="s">
+      <c r="A30" s="63"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="74"/>
+      <c r="H30" s="75"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="75"/>
+      <c r="J30" s="76"/>
       <c r="L30" s="4"/>
       <c r="M30" s="18"/>
       <c r="N30" s="4"/>
@@ -4256,18 +4184,18 @@
       <c r="Q30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="55" t="s">
+      <c r="A31" s="63"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="74"/>
+      <c r="H31" s="75"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="75"/>
+      <c r="J31" s="76"/>
       <c r="L31" s="4"/>
       <c r="M31" s="18"/>
       <c r="N31" s="4"/>
@@ -4276,18 +4204,18 @@
       <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="55" t="s">
+      <c r="A32" s="63"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="74"/>
+      <c r="H32" s="75"/>
       <c r="I32" s="21"/>
-      <c r="J32" s="75"/>
+      <c r="J32" s="76"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -4297,20 +4225,20 @@
       <c r="Q32" s="4"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="71"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="72"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="30"/>
+      <c r="J33" s="31"/>
       <c r="K33" s="13"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -4320,1217 +4248,1217 @@
       <c r="Q33" s="4"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="63" t="s">
+      <c r="A34" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
       <c r="I34" s="20"/>
-      <c r="J34" s="30"/>
+      <c r="J34" s="31"/>
       <c r="K34" s="13"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="59" t="s">
+      <c r="A35" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="76"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="77"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="78"/>
       <c r="K35" s="13"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="81" t="s">
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="F36" s="81" t="s">
+      <c r="F36" s="82" t="s">
         <v>234</v>
       </c>
-      <c r="G36" s="81" t="s">
+      <c r="G36" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="H36" s="44" t="s">
+      <c r="H36" s="45" t="s">
         <v>19</v>
       </c>
       <c r="I36" s="20"/>
-      <c r="J36" s="30"/>
+      <c r="J36" s="31"/>
       <c r="K36" s="13"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="80" t="s">
+      <c r="A37" s="60"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="I37" s="31"/>
-      <c r="J37" s="77"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="78"/>
       <c r="K37" s="13"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="64" t="s">
+      <c r="A38" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="69"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="67"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="70"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="71"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="56" t="s">
         <v>96</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="72"/>
       <c r="I39" s="20"/>
-      <c r="J39" s="30"/>
+      <c r="J39" s="31"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="56" t="s">
         <v>97</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
-      <c r="D40" s="74"/>
-      <c r="E40" s="74"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="74"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
       <c r="I40" s="21"/>
-      <c r="J40" s="75"/>
+      <c r="J40" s="76"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="55" t="s">
+      <c r="A41" s="56" t="s">
         <v>98</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
       <c r="I41" s="21"/>
-      <c r="J41" s="75"/>
+      <c r="J41" s="76"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="56" t="s">
         <v>99</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="75"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
       <c r="I42" s="21"/>
-      <c r="J42" s="75"/>
+      <c r="J42" s="76"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="56" t="s">
         <v>100</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="74"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
       <c r="I43" s="21"/>
-      <c r="J43" s="75"/>
+      <c r="J43" s="76"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="56" t="s">
         <v>101</v>
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="74"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="75"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="75"/>
+      <c r="H44" s="75"/>
       <c r="I44" s="21"/>
-      <c r="J44" s="75"/>
+      <c r="J44" s="76"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="55" t="s">
+      <c r="A45" s="56" t="s">
         <v>102</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="75"/>
+      <c r="H45" s="75"/>
       <c r="I45" s="21"/>
-      <c r="J45" s="75"/>
+      <c r="J45" s="76"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+      <c r="A46" s="56" t="s">
         <v>103</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="74"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="75"/>
+      <c r="H46" s="75"/>
       <c r="I46" s="21"/>
-      <c r="J46" s="75"/>
+      <c r="J46" s="76"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="55" t="s">
+      <c r="A47" s="56" t="s">
         <v>104</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="74"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="75"/>
+      <c r="J47" s="76"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="55" t="s">
+      <c r="A48" s="56" t="s">
         <v>105</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="74"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="75"/>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="75"/>
+      <c r="J48" s="76"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="56" t="s">
         <v>106</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
       <c r="I49" s="21"/>
-      <c r="J49" s="75"/>
+      <c r="J49" s="76"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="55" t="s">
+      <c r="A50" s="56" t="s">
         <v>107</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
       <c r="I50" s="21"/>
-      <c r="J50" s="75"/>
+      <c r="J50" s="76"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="55" t="s">
+      <c r="A51" s="56" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="74"/>
-      <c r="H51" s="74"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="75"/>
+      <c r="F51" s="75"/>
+      <c r="G51" s="75"/>
+      <c r="H51" s="75"/>
       <c r="I51" s="21"/>
-      <c r="J51" s="75"/>
+      <c r="J51" s="76"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="55" t="s">
+      <c r="A52" s="56" t="s">
         <v>109</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="74"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
       <c r="I52" s="21"/>
-      <c r="J52" s="75"/>
+      <c r="J52" s="76"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="55" t="s">
+      <c r="A53" s="56" t="s">
         <v>110</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
-      <c r="D53" s="74"/>
-      <c r="E53" s="74"/>
-      <c r="F53" s="74"/>
-      <c r="G53" s="74"/>
-      <c r="H53" s="74"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="75"/>
+      <c r="F53" s="75"/>
+      <c r="G53" s="75"/>
+      <c r="H53" s="75"/>
       <c r="I53" s="21"/>
-      <c r="J53" s="75"/>
+      <c r="J53" s="76"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="55" t="s">
+      <c r="A54" s="56" t="s">
         <v>111</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="74"/>
-      <c r="H54" s="74"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="75"/>
+      <c r="F54" s="75"/>
+      <c r="G54" s="75"/>
+      <c r="H54" s="75"/>
       <c r="I54" s="21"/>
-      <c r="J54" s="75"/>
+      <c r="J54" s="76"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="65" t="s">
+      <c r="A55" s="66" t="s">
         <v>112</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
-      <c r="D55" s="74"/>
-      <c r="E55" s="74"/>
-      <c r="F55" s="74"/>
-      <c r="G55" s="74"/>
-      <c r="H55" s="74"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="75"/>
       <c r="I55" s="21"/>
-      <c r="J55" s="75"/>
+      <c r="J55" s="76"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="65" t="s">
+      <c r="A56" s="66" t="s">
         <v>113</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="74"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="75"/>
+      <c r="F56" s="75"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="75"/>
       <c r="I56" s="21"/>
-      <c r="J56" s="75"/>
+      <c r="J56" s="76"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="65" t="s">
+      <c r="A57" s="66" t="s">
         <v>114</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="74"/>
-      <c r="F57" s="74"/>
-      <c r="G57" s="74"/>
-      <c r="H57" s="74"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="75"/>
+      <c r="F57" s="75"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="75"/>
       <c r="I57" s="21"/>
-      <c r="J57" s="75"/>
+      <c r="J57" s="76"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="65" t="s">
+      <c r="A58" s="66" t="s">
         <v>115</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="74"/>
-      <c r="H58" s="74"/>
+      <c r="D58" s="75"/>
+      <c r="E58" s="75"/>
+      <c r="F58" s="75"/>
+      <c r="G58" s="75"/>
+      <c r="H58" s="75"/>
       <c r="I58" s="21"/>
-      <c r="J58" s="75"/>
+      <c r="J58" s="76"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="65" t="s">
+      <c r="A59" s="66" t="s">
         <v>116</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
-      <c r="D59" s="74"/>
-      <c r="E59" s="74"/>
-      <c r="F59" s="74"/>
-      <c r="G59" s="74"/>
-      <c r="H59" s="74"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="75"/>
+      <c r="F59" s="75"/>
+      <c r="G59" s="75"/>
+      <c r="H59" s="75"/>
       <c r="I59" s="21"/>
-      <c r="J59" s="75"/>
+      <c r="J59" s="76"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="65" t="s">
+      <c r="A60" s="66" t="s">
         <v>117</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
-      <c r="D60" s="74"/>
-      <c r="E60" s="74"/>
-      <c r="F60" s="74"/>
-      <c r="G60" s="74"/>
-      <c r="H60" s="74"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="75"/>
+      <c r="F60" s="75"/>
+      <c r="G60" s="75"/>
+      <c r="H60" s="75"/>
       <c r="I60" s="21"/>
-      <c r="J60" s="75"/>
+      <c r="J60" s="76"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="65" t="s">
+      <c r="A61" s="66" t="s">
         <v>118</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="21"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-      <c r="G61" s="74"/>
-      <c r="H61" s="74"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="75"/>
+      <c r="F61" s="75"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="75"/>
       <c r="I61" s="21"/>
-      <c r="J61" s="75"/>
+      <c r="J61" s="76"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="65" t="s">
+      <c r="A62" s="66" t="s">
         <v>119</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
-      <c r="D62" s="74"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="74"/>
-      <c r="G62" s="74"/>
-      <c r="H62" s="74"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="75"/>
+      <c r="F62" s="75"/>
+      <c r="G62" s="75"/>
+      <c r="H62" s="75"/>
       <c r="I62" s="21"/>
-      <c r="J62" s="75"/>
+      <c r="J62" s="76"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="65" t="s">
+      <c r="A63" s="66" t="s">
         <v>120</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
-      <c r="F63" s="74"/>
-      <c r="G63" s="74"/>
-      <c r="H63" s="74"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
+      <c r="F63" s="75"/>
+      <c r="G63" s="75"/>
+      <c r="H63" s="75"/>
       <c r="I63" s="21"/>
-      <c r="J63" s="75"/>
+      <c r="J63" s="76"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="65" t="s">
+      <c r="A64" s="66" t="s">
         <v>121</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
-      <c r="F64" s="74"/>
-      <c r="G64" s="74"/>
-      <c r="H64" s="74"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="75"/>
+      <c r="F64" s="75"/>
+      <c r="G64" s="75"/>
+      <c r="H64" s="75"/>
       <c r="I64" s="21"/>
-      <c r="J64" s="75"/>
+      <c r="J64" s="76"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="65" t="s">
+      <c r="A65" s="66" t="s">
         <v>122</v>
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
-      <c r="F65" s="74"/>
-      <c r="G65" s="74"/>
-      <c r="H65" s="74"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="75"/>
+      <c r="F65" s="75"/>
+      <c r="G65" s="75"/>
+      <c r="H65" s="75"/>
       <c r="I65" s="21"/>
-      <c r="J65" s="75"/>
+      <c r="J65" s="76"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="65" t="s">
+      <c r="A66" s="66" t="s">
         <v>123</v>
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="21"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="74"/>
-      <c r="H66" s="74"/>
+      <c r="D66" s="75"/>
+      <c r="E66" s="75"/>
+      <c r="F66" s="75"/>
+      <c r="G66" s="75"/>
+      <c r="H66" s="75"/>
       <c r="I66" s="21"/>
-      <c r="J66" s="75"/>
+      <c r="J66" s="76"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="65" t="s">
+      <c r="A67" s="66" t="s">
         <v>124</v>
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="74"/>
-      <c r="H67" s="74"/>
+      <c r="D67" s="75"/>
+      <c r="E67" s="75"/>
+      <c r="F67" s="75"/>
+      <c r="G67" s="75"/>
+      <c r="H67" s="75"/>
       <c r="I67" s="21"/>
-      <c r="J67" s="75"/>
+      <c r="J67" s="76"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="65" t="s">
+      <c r="A68" s="66" t="s">
         <v>125</v>
       </c>
       <c r="B68" s="21"/>
       <c r="C68" s="21"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="74"/>
-      <c r="H68" s="74"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="75"/>
+      <c r="F68" s="75"/>
+      <c r="G68" s="75"/>
+      <c r="H68" s="75"/>
       <c r="I68" s="21"/>
-      <c r="J68" s="75"/>
+      <c r="J68" s="76"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="65" t="s">
+      <c r="A69" s="66" t="s">
         <v>126</v>
       </c>
       <c r="B69" s="21"/>
       <c r="C69" s="21"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
-      <c r="F69" s="74"/>
-      <c r="G69" s="74"/>
-      <c r="H69" s="74"/>
+      <c r="D69" s="75"/>
+      <c r="E69" s="75"/>
+      <c r="F69" s="75"/>
+      <c r="G69" s="75"/>
+      <c r="H69" s="75"/>
       <c r="I69" s="21"/>
-      <c r="J69" s="75"/>
+      <c r="J69" s="76"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="65" t="s">
+      <c r="A70" s="66" t="s">
         <v>127</v>
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="75"/>
+      <c r="F70" s="75"/>
+      <c r="G70" s="75"/>
+      <c r="H70" s="75"/>
       <c r="I70" s="21"/>
-      <c r="J70" s="75"/>
+      <c r="J70" s="76"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="65" t="s">
+      <c r="A71" s="66" t="s">
         <v>128</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="21"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="74"/>
-      <c r="F71" s="74"/>
-      <c r="G71" s="74"/>
-      <c r="H71" s="74"/>
+      <c r="D71" s="75"/>
+      <c r="E71" s="75"/>
+      <c r="F71" s="75"/>
+      <c r="G71" s="75"/>
+      <c r="H71" s="75"/>
       <c r="I71" s="21"/>
-      <c r="J71" s="75"/>
+      <c r="J71" s="76"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="65" t="s">
+      <c r="A72" s="66" t="s">
         <v>129</v>
       </c>
       <c r="B72" s="21"/>
       <c r="C72" s="21"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="74"/>
-      <c r="H72" s="74"/>
+      <c r="D72" s="75"/>
+      <c r="E72" s="75"/>
+      <c r="F72" s="75"/>
+      <c r="G72" s="75"/>
+      <c r="H72" s="75"/>
       <c r="I72" s="21"/>
-      <c r="J72" s="75"/>
+      <c r="J72" s="76"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="65" t="s">
+      <c r="A73" s="66" t="s">
         <v>130</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="74"/>
-      <c r="H73" s="74"/>
+      <c r="D73" s="75"/>
+      <c r="E73" s="75"/>
+      <c r="F73" s="75"/>
+      <c r="G73" s="75"/>
+      <c r="H73" s="75"/>
       <c r="I73" s="21"/>
-      <c r="J73" s="75"/>
+      <c r="J73" s="76"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="65" t="s">
+      <c r="A74" s="66" t="s">
         <v>131</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="74"/>
-      <c r="H74" s="74"/>
+      <c r="D74" s="75"/>
+      <c r="E74" s="75"/>
+      <c r="F74" s="75"/>
+      <c r="G74" s="75"/>
+      <c r="H74" s="75"/>
       <c r="I74" s="21"/>
-      <c r="J74" s="75"/>
+      <c r="J74" s="76"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="65" t="s">
+      <c r="A75" s="66" t="s">
         <v>132</v>
       </c>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="74"/>
-      <c r="H75" s="74"/>
+      <c r="D75" s="75"/>
+      <c r="E75" s="75"/>
+      <c r="F75" s="75"/>
+      <c r="G75" s="75"/>
+      <c r="H75" s="75"/>
       <c r="I75" s="21"/>
-      <c r="J75" s="75"/>
+      <c r="J75" s="76"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="65" t="s">
+      <c r="A76" s="66" t="s">
         <v>133</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="74"/>
-      <c r="H76" s="74"/>
+      <c r="D76" s="75"/>
+      <c r="E76" s="75"/>
+      <c r="F76" s="75"/>
+      <c r="G76" s="75"/>
+      <c r="H76" s="75"/>
       <c r="I76" s="21"/>
-      <c r="J76" s="75"/>
+      <c r="J76" s="76"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="65" t="s">
+      <c r="A77" s="66" t="s">
         <v>134</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="74"/>
-      <c r="H77" s="74"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="75"/>
+      <c r="F77" s="75"/>
+      <c r="G77" s="75"/>
+      <c r="H77" s="75"/>
       <c r="I77" s="21"/>
-      <c r="J77" s="75"/>
+      <c r="J77" s="76"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="65" t="s">
+      <c r="A78" s="66" t="s">
         <v>135</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="74"/>
-      <c r="H78" s="74"/>
+      <c r="D78" s="75"/>
+      <c r="E78" s="75"/>
+      <c r="F78" s="75"/>
+      <c r="G78" s="75"/>
+      <c r="H78" s="75"/>
       <c r="I78" s="21"/>
-      <c r="J78" s="75"/>
+      <c r="J78" s="76"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="65" t="s">
+      <c r="A79" s="66" t="s">
         <v>136</v>
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="74"/>
-      <c r="H79" s="74"/>
+      <c r="D79" s="75"/>
+      <c r="E79" s="75"/>
+      <c r="F79" s="75"/>
+      <c r="G79" s="75"/>
+      <c r="H79" s="75"/>
       <c r="I79" s="21"/>
-      <c r="J79" s="75"/>
+      <c r="J79" s="76"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="65" t="s">
+      <c r="A80" s="66" t="s">
         <v>137</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="21"/>
-      <c r="D80" s="74"/>
-      <c r="E80" s="74"/>
-      <c r="F80" s="74"/>
-      <c r="G80" s="74"/>
-      <c r="H80" s="74"/>
+      <c r="D80" s="75"/>
+      <c r="E80" s="75"/>
+      <c r="F80" s="75"/>
+      <c r="G80" s="75"/>
+      <c r="H80" s="75"/>
       <c r="I80" s="21"/>
-      <c r="J80" s="75"/>
+      <c r="J80" s="76"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="65" t="s">
+      <c r="A81" s="66" t="s">
         <v>138</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
-      <c r="D81" s="74"/>
-      <c r="E81" s="74"/>
-      <c r="F81" s="74"/>
-      <c r="G81" s="74"/>
-      <c r="H81" s="74"/>
+      <c r="D81" s="75"/>
+      <c r="E81" s="75"/>
+      <c r="F81" s="75"/>
+      <c r="G81" s="75"/>
+      <c r="H81" s="75"/>
       <c r="I81" s="21"/>
-      <c r="J81" s="75"/>
+      <c r="J81" s="76"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="65" t="s">
+      <c r="A82" s="66" t="s">
         <v>139</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="21"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="74"/>
-      <c r="F82" s="74"/>
-      <c r="G82" s="74"/>
-      <c r="H82" s="74"/>
+      <c r="D82" s="75"/>
+      <c r="E82" s="75"/>
+      <c r="F82" s="75"/>
+      <c r="G82" s="75"/>
+      <c r="H82" s="75"/>
       <c r="I82" s="21"/>
-      <c r="J82" s="75"/>
+      <c r="J82" s="76"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="65" t="s">
+      <c r="A83" s="66" t="s">
         <v>140</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="21"/>
-      <c r="D83" s="74"/>
-      <c r="E83" s="74"/>
-      <c r="F83" s="74"/>
-      <c r="G83" s="74"/>
-      <c r="H83" s="74"/>
+      <c r="D83" s="75"/>
+      <c r="E83" s="75"/>
+      <c r="F83" s="75"/>
+      <c r="G83" s="75"/>
+      <c r="H83" s="75"/>
       <c r="I83" s="21"/>
-      <c r="J83" s="75"/>
+      <c r="J83" s="76"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="65" t="s">
+      <c r="A84" s="66" t="s">
         <v>141</v>
       </c>
       <c r="B84" s="21"/>
       <c r="C84" s="21"/>
-      <c r="D84" s="74"/>
-      <c r="E84" s="74"/>
-      <c r="F84" s="74"/>
-      <c r="G84" s="74"/>
-      <c r="H84" s="74"/>
+      <c r="D84" s="75"/>
+      <c r="E84" s="75"/>
+      <c r="F84" s="75"/>
+      <c r="G84" s="75"/>
+      <c r="H84" s="75"/>
       <c r="I84" s="21"/>
-      <c r="J84" s="75"/>
+      <c r="J84" s="76"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="65" t="s">
+      <c r="A85" s="66" t="s">
         <v>142</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
-      <c r="D85" s="74"/>
-      <c r="E85" s="74"/>
-      <c r="F85" s="74"/>
-      <c r="G85" s="74"/>
-      <c r="H85" s="74"/>
+      <c r="D85" s="75"/>
+      <c r="E85" s="75"/>
+      <c r="F85" s="75"/>
+      <c r="G85" s="75"/>
+      <c r="H85" s="75"/>
       <c r="I85" s="21"/>
-      <c r="J85" s="75"/>
+      <c r="J85" s="76"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="65" t="s">
+      <c r="A86" s="66" t="s">
         <v>143</v>
       </c>
       <c r="B86" s="21"/>
       <c r="C86" s="21"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="74"/>
-      <c r="G86" s="74"/>
-      <c r="H86" s="74"/>
+      <c r="D86" s="75"/>
+      <c r="E86" s="75"/>
+      <c r="F86" s="75"/>
+      <c r="G86" s="75"/>
+      <c r="H86" s="75"/>
       <c r="I86" s="21"/>
-      <c r="J86" s="75"/>
+      <c r="J86" s="76"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="65" t="s">
+      <c r="A87" s="66" t="s">
         <v>144</v>
       </c>
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
-      <c r="D87" s="74"/>
-      <c r="E87" s="74"/>
-      <c r="F87" s="74"/>
-      <c r="G87" s="74"/>
-      <c r="H87" s="74"/>
+      <c r="D87" s="75"/>
+      <c r="E87" s="75"/>
+      <c r="F87" s="75"/>
+      <c r="G87" s="75"/>
+      <c r="H87" s="75"/>
       <c r="I87" s="21"/>
-      <c r="J87" s="75"/>
+      <c r="J87" s="76"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="65" t="s">
+      <c r="A88" s="66" t="s">
         <v>145</v>
       </c>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
-      <c r="D88" s="74"/>
-      <c r="E88" s="74"/>
-      <c r="F88" s="74"/>
-      <c r="G88" s="74"/>
-      <c r="H88" s="74"/>
+      <c r="D88" s="75"/>
+      <c r="E88" s="75"/>
+      <c r="F88" s="75"/>
+      <c r="G88" s="75"/>
+      <c r="H88" s="75"/>
       <c r="I88" s="21"/>
-      <c r="J88" s="75"/>
+      <c r="J88" s="76"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="65" t="s">
+      <c r="A89" s="66" t="s">
         <v>146</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
-      <c r="D89" s="74"/>
-      <c r="E89" s="74"/>
-      <c r="F89" s="74"/>
-      <c r="G89" s="74"/>
-      <c r="H89" s="74"/>
+      <c r="D89" s="75"/>
+      <c r="E89" s="75"/>
+      <c r="F89" s="75"/>
+      <c r="G89" s="75"/>
+      <c r="H89" s="75"/>
       <c r="I89" s="21"/>
-      <c r="J89" s="75"/>
+      <c r="J89" s="76"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="65" t="s">
+      <c r="A90" s="66" t="s">
         <v>147</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
-      <c r="D90" s="74"/>
-      <c r="E90" s="74"/>
-      <c r="F90" s="74"/>
-      <c r="G90" s="74"/>
-      <c r="H90" s="74"/>
+      <c r="D90" s="75"/>
+      <c r="E90" s="75"/>
+      <c r="F90" s="75"/>
+      <c r="G90" s="75"/>
+      <c r="H90" s="75"/>
       <c r="I90" s="21"/>
-      <c r="J90" s="75"/>
+      <c r="J90" s="76"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="65" t="s">
+      <c r="A91" s="66" t="s">
         <v>148</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
-      <c r="D91" s="74"/>
-      <c r="E91" s="74"/>
-      <c r="F91" s="74"/>
-      <c r="G91" s="74"/>
-      <c r="H91" s="74"/>
+      <c r="D91" s="75"/>
+      <c r="E91" s="75"/>
+      <c r="F91" s="75"/>
+      <c r="G91" s="75"/>
+      <c r="H91" s="75"/>
       <c r="I91" s="21"/>
-      <c r="J91" s="75"/>
+      <c r="J91" s="76"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="65" t="s">
+      <c r="A92" s="66" t="s">
         <v>149</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="21"/>
-      <c r="D92" s="74"/>
-      <c r="E92" s="74"/>
-      <c r="F92" s="74"/>
-      <c r="G92" s="74"/>
-      <c r="H92" s="74"/>
+      <c r="D92" s="75"/>
+      <c r="E92" s="75"/>
+      <c r="F92" s="75"/>
+      <c r="G92" s="75"/>
+      <c r="H92" s="75"/>
       <c r="I92" s="21"/>
-      <c r="J92" s="75"/>
+      <c r="J92" s="76"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="65" t="s">
+      <c r="A93" s="66" t="s">
         <v>150</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="21"/>
-      <c r="D93" s="74"/>
-      <c r="E93" s="74"/>
-      <c r="F93" s="74"/>
-      <c r="G93" s="74"/>
-      <c r="H93" s="74"/>
+      <c r="D93" s="75"/>
+      <c r="E93" s="75"/>
+      <c r="F93" s="75"/>
+      <c r="G93" s="75"/>
+      <c r="H93" s="75"/>
       <c r="I93" s="21"/>
-      <c r="J93" s="75"/>
+      <c r="J93" s="76"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="65" t="s">
+      <c r="A94" s="66" t="s">
         <v>151</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
-      <c r="D94" s="74"/>
-      <c r="E94" s="74"/>
-      <c r="F94" s="74"/>
-      <c r="G94" s="74"/>
-      <c r="H94" s="74"/>
+      <c r="D94" s="75"/>
+      <c r="E94" s="75"/>
+      <c r="F94" s="75"/>
+      <c r="G94" s="75"/>
+      <c r="H94" s="75"/>
       <c r="I94" s="21"/>
-      <c r="J94" s="75"/>
+      <c r="J94" s="76"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="65" t="s">
+      <c r="A95" s="66" t="s">
         <v>152</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="21"/>
-      <c r="D95" s="74"/>
-      <c r="E95" s="74"/>
-      <c r="F95" s="74"/>
-      <c r="G95" s="74"/>
-      <c r="H95" s="74"/>
+      <c r="D95" s="75"/>
+      <c r="E95" s="75"/>
+      <c r="F95" s="75"/>
+      <c r="G95" s="75"/>
+      <c r="H95" s="75"/>
       <c r="I95" s="21"/>
-      <c r="J95" s="75"/>
+      <c r="J95" s="76"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="65" t="s">
+      <c r="A96" s="66" t="s">
         <v>153</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="21"/>
-      <c r="D96" s="74"/>
-      <c r="E96" s="74"/>
-      <c r="F96" s="74"/>
-      <c r="G96" s="74"/>
-      <c r="H96" s="74"/>
+      <c r="D96" s="75"/>
+      <c r="E96" s="75"/>
+      <c r="F96" s="75"/>
+      <c r="G96" s="75"/>
+      <c r="H96" s="75"/>
       <c r="I96" s="21"/>
-      <c r="J96" s="75"/>
+      <c r="J96" s="76"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="65" t="s">
+      <c r="A97" s="66" t="s">
         <v>154</v>
       </c>
       <c r="B97" s="21"/>
       <c r="C97" s="21"/>
-      <c r="D97" s="74"/>
-      <c r="E97" s="74"/>
-      <c r="F97" s="74"/>
-      <c r="G97" s="74"/>
-      <c r="H97" s="74"/>
+      <c r="D97" s="75"/>
+      <c r="E97" s="75"/>
+      <c r="F97" s="75"/>
+      <c r="G97" s="75"/>
+      <c r="H97" s="75"/>
       <c r="I97" s="21"/>
-      <c r="J97" s="75"/>
+      <c r="J97" s="76"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="65" t="s">
+      <c r="A98" s="66" t="s">
         <v>155</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="21"/>
-      <c r="D98" s="74"/>
-      <c r="E98" s="74"/>
-      <c r="F98" s="74"/>
-      <c r="G98" s="74"/>
-      <c r="H98" s="74"/>
+      <c r="D98" s="75"/>
+      <c r="E98" s="75"/>
+      <c r="F98" s="75"/>
+      <c r="G98" s="75"/>
+      <c r="H98" s="75"/>
       <c r="I98" s="21"/>
-      <c r="J98" s="75"/>
+      <c r="J98" s="76"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="65" t="s">
+      <c r="A99" s="66" t="s">
         <v>156</v>
       </c>
       <c r="B99" s="21"/>
       <c r="C99" s="21"/>
-      <c r="D99" s="74"/>
-      <c r="E99" s="74"/>
-      <c r="F99" s="74"/>
-      <c r="G99" s="74"/>
-      <c r="H99" s="74"/>
+      <c r="D99" s="75"/>
+      <c r="E99" s="75"/>
+      <c r="F99" s="75"/>
+      <c r="G99" s="75"/>
+      <c r="H99" s="75"/>
       <c r="I99" s="21"/>
-      <c r="J99" s="75"/>
+      <c r="J99" s="76"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="65" t="s">
+      <c r="A100" s="66" t="s">
         <v>157</v>
       </c>
       <c r="B100" s="21"/>
       <c r="C100" s="21"/>
-      <c r="D100" s="74"/>
-      <c r="E100" s="74"/>
-      <c r="F100" s="74"/>
-      <c r="G100" s="74"/>
-      <c r="H100" s="74"/>
+      <c r="D100" s="75"/>
+      <c r="E100" s="75"/>
+      <c r="F100" s="75"/>
+      <c r="G100" s="75"/>
+      <c r="H100" s="75"/>
       <c r="I100" s="21"/>
-      <c r="J100" s="75"/>
+      <c r="J100" s="76"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="65" t="s">
+      <c r="A101" s="66" t="s">
         <v>158</v>
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="21"/>
-      <c r="D101" s="74"/>
-      <c r="E101" s="74"/>
-      <c r="F101" s="74"/>
-      <c r="G101" s="74"/>
-      <c r="H101" s="74"/>
+      <c r="D101" s="75"/>
+      <c r="E101" s="75"/>
+      <c r="F101" s="75"/>
+      <c r="G101" s="75"/>
+      <c r="H101" s="75"/>
       <c r="I101" s="21"/>
-      <c r="J101" s="75"/>
+      <c r="J101" s="76"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="65" t="s">
+      <c r="A102" s="66" t="s">
         <v>159</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="21"/>
-      <c r="D102" s="74"/>
-      <c r="E102" s="74"/>
-      <c r="F102" s="74"/>
-      <c r="G102" s="74"/>
-      <c r="H102" s="74"/>
+      <c r="D102" s="75"/>
+      <c r="E102" s="75"/>
+      <c r="F102" s="75"/>
+      <c r="G102" s="75"/>
+      <c r="H102" s="75"/>
       <c r="I102" s="21"/>
-      <c r="J102" s="75"/>
+      <c r="J102" s="76"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="65" t="s">
+      <c r="A103" s="66" t="s">
         <v>160</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="21"/>
-      <c r="D103" s="74"/>
-      <c r="E103" s="74"/>
-      <c r="F103" s="74"/>
-      <c r="G103" s="74"/>
-      <c r="H103" s="74"/>
+      <c r="D103" s="75"/>
+      <c r="E103" s="75"/>
+      <c r="F103" s="75"/>
+      <c r="G103" s="75"/>
+      <c r="H103" s="75"/>
       <c r="I103" s="21"/>
-      <c r="J103" s="75"/>
+      <c r="J103" s="76"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="65" t="s">
+      <c r="A104" s="66" t="s">
         <v>161</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="21"/>
-      <c r="D104" s="74"/>
-      <c r="E104" s="74"/>
-      <c r="F104" s="74"/>
-      <c r="G104" s="74"/>
-      <c r="H104" s="74"/>
+      <c r="D104" s="75"/>
+      <c r="E104" s="75"/>
+      <c r="F104" s="75"/>
+      <c r="G104" s="75"/>
+      <c r="H104" s="75"/>
       <c r="I104" s="21"/>
-      <c r="J104" s="75"/>
+      <c r="J104" s="76"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="65" t="s">
+      <c r="A105" s="66" t="s">
         <v>162</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="21"/>
-      <c r="D105" s="74"/>
-      <c r="E105" s="74"/>
-      <c r="F105" s="74"/>
-      <c r="G105" s="74"/>
-      <c r="H105" s="74"/>
+      <c r="D105" s="75"/>
+      <c r="E105" s="75"/>
+      <c r="F105" s="75"/>
+      <c r="G105" s="75"/>
+      <c r="H105" s="75"/>
       <c r="I105" s="21"/>
-      <c r="J105" s="75"/>
+      <c r="J105" s="76"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="65" t="s">
+      <c r="A106" s="66" t="s">
         <v>163</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="21"/>
-      <c r="D106" s="74"/>
-      <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
-      <c r="G106" s="74"/>
-      <c r="H106" s="74"/>
+      <c r="D106" s="75"/>
+      <c r="E106" s="75"/>
+      <c r="F106" s="75"/>
+      <c r="G106" s="75"/>
+      <c r="H106" s="75"/>
       <c r="I106" s="21"/>
-      <c r="J106" s="75"/>
+      <c r="J106" s="76"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="65" t="s">
+      <c r="A107" s="66" t="s">
         <v>164</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="21"/>
-      <c r="D107" s="74"/>
-      <c r="E107" s="74"/>
-      <c r="F107" s="74"/>
-      <c r="G107" s="74"/>
-      <c r="H107" s="74"/>
+      <c r="D107" s="75"/>
+      <c r="E107" s="75"/>
+      <c r="F107" s="75"/>
+      <c r="G107" s="75"/>
+      <c r="H107" s="75"/>
       <c r="I107" s="21"/>
-      <c r="J107" s="75"/>
+      <c r="J107" s="76"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="65" t="s">
+      <c r="A108" s="66" t="s">
         <v>165</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="21"/>
-      <c r="D108" s="74"/>
-      <c r="E108" s="74"/>
-      <c r="F108" s="74"/>
-      <c r="G108" s="74"/>
-      <c r="H108" s="74"/>
+      <c r="D108" s="75"/>
+      <c r="E108" s="75"/>
+      <c r="F108" s="75"/>
+      <c r="G108" s="75"/>
+      <c r="H108" s="75"/>
       <c r="I108" s="21"/>
-      <c r="J108" s="75"/>
+      <c r="J108" s="76"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="65" t="s">
+      <c r="A109" s="66" t="s">
         <v>166</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="21"/>
-      <c r="D109" s="74"/>
-      <c r="E109" s="74"/>
-      <c r="F109" s="74"/>
-      <c r="G109" s="74"/>
-      <c r="H109" s="74"/>
+      <c r="D109" s="75"/>
+      <c r="E109" s="75"/>
+      <c r="F109" s="75"/>
+      <c r="G109" s="75"/>
+      <c r="H109" s="75"/>
       <c r="I109" s="21"/>
-      <c r="J109" s="75"/>
+      <c r="J109" s="76"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="65" t="s">
+      <c r="A110" s="66" t="s">
         <v>167</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="21"/>
-      <c r="D110" s="74"/>
-      <c r="E110" s="74"/>
-      <c r="F110" s="74"/>
-      <c r="G110" s="74"/>
-      <c r="H110" s="74"/>
+      <c r="D110" s="75"/>
+      <c r="E110" s="75"/>
+      <c r="F110" s="75"/>
+      <c r="G110" s="75"/>
+      <c r="H110" s="75"/>
       <c r="I110" s="21"/>
-      <c r="J110" s="75"/>
+      <c r="J110" s="76"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="65" t="s">
+      <c r="A111" s="66" t="s">
         <v>168</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="21"/>
-      <c r="D111" s="74"/>
-      <c r="E111" s="74"/>
-      <c r="F111" s="74"/>
-      <c r="G111" s="74"/>
-      <c r="H111" s="74"/>
+      <c r="D111" s="75"/>
+      <c r="E111" s="75"/>
+      <c r="F111" s="75"/>
+      <c r="G111" s="75"/>
+      <c r="H111" s="75"/>
       <c r="I111" s="21"/>
-      <c r="J111" s="75"/>
+      <c r="J111" s="76"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="65" t="s">
+      <c r="A112" s="66" t="s">
         <v>169</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="21"/>
-      <c r="D112" s="74"/>
-      <c r="E112" s="74"/>
-      <c r="F112" s="74"/>
-      <c r="G112" s="74"/>
-      <c r="H112" s="74"/>
+      <c r="D112" s="75"/>
+      <c r="E112" s="75"/>
+      <c r="F112" s="75"/>
+      <c r="G112" s="75"/>
+      <c r="H112" s="75"/>
       <c r="I112" s="21"/>
-      <c r="J112" s="75"/>
+      <c r="J112" s="76"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="65" t="s">
+      <c r="A113" s="66" t="s">
         <v>170</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="21"/>
-      <c r="D113" s="74"/>
-      <c r="E113" s="74"/>
-      <c r="F113" s="74"/>
-      <c r="G113" s="74"/>
-      <c r="H113" s="74"/>
+      <c r="D113" s="75"/>
+      <c r="E113" s="75"/>
+      <c r="F113" s="75"/>
+      <c r="G113" s="75"/>
+      <c r="H113" s="75"/>
       <c r="I113" s="21"/>
-      <c r="J113" s="75"/>
+      <c r="J113" s="76"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="65" t="s">
+      <c r="A114" s="66" t="s">
         <v>171</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="21"/>
-      <c r="D114" s="74"/>
-      <c r="E114" s="74"/>
-      <c r="F114" s="74"/>
-      <c r="G114" s="74"/>
-      <c r="H114" s="74"/>
+      <c r="D114" s="75"/>
+      <c r="E114" s="75"/>
+      <c r="F114" s="75"/>
+      <c r="G114" s="75"/>
+      <c r="H114" s="75"/>
       <c r="I114" s="21"/>
-      <c r="J114" s="75"/>
+      <c r="J114" s="76"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="65" t="s">
+      <c r="A115" s="66" t="s">
         <v>172</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="21"/>
-      <c r="D115" s="74"/>
-      <c r="E115" s="74"/>
-      <c r="F115" s="74"/>
-      <c r="G115" s="74"/>
-      <c r="H115" s="74"/>
+      <c r="D115" s="75"/>
+      <c r="E115" s="75"/>
+      <c r="F115" s="75"/>
+      <c r="G115" s="75"/>
+      <c r="H115" s="75"/>
       <c r="I115" s="21"/>
-      <c r="J115" s="75"/>
+      <c r="J115" s="76"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="65" t="s">
+      <c r="A116" s="66" t="s">
         <v>173</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="21"/>
-      <c r="D116" s="74"/>
-      <c r="E116" s="74"/>
-      <c r="F116" s="74"/>
-      <c r="G116" s="74"/>
-      <c r="H116" s="74"/>
+      <c r="D116" s="75"/>
+      <c r="E116" s="75"/>
+      <c r="F116" s="75"/>
+      <c r="G116" s="75"/>
+      <c r="H116" s="75"/>
       <c r="I116" s="21"/>
-      <c r="J116" s="75"/>
+      <c r="J116" s="76"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="65" t="s">
+      <c r="A117" s="66" t="s">
         <v>174</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="21"/>
-      <c r="D117" s="74"/>
-      <c r="E117" s="74"/>
-      <c r="F117" s="74"/>
-      <c r="G117" s="74"/>
-      <c r="H117" s="74"/>
+      <c r="D117" s="75"/>
+      <c r="E117" s="75"/>
+      <c r="F117" s="75"/>
+      <c r="G117" s="75"/>
+      <c r="H117" s="75"/>
       <c r="I117" s="21"/>
-      <c r="J117" s="75"/>
+      <c r="J117" s="76"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="66" t="s">
+      <c r="A118" s="67" t="s">
         <v>175</v>
       </c>
-      <c r="B118" s="31"/>
-      <c r="C118" s="31"/>
-      <c r="D118" s="76"/>
-      <c r="E118" s="76"/>
-      <c r="F118" s="76"/>
-      <c r="G118" s="76"/>
-      <c r="H118" s="76"/>
-      <c r="I118" s="31"/>
-      <c r="J118" s="77"/>
+      <c r="B118" s="32"/>
+      <c r="C118" s="32"/>
+      <c r="D118" s="77"/>
+      <c r="E118" s="77"/>
+      <c r="F118" s="77"/>
+      <c r="G118" s="77"/>
+      <c r="H118" s="77"/>
+      <c r="I118" s="32"/>
+      <c r="J118" s="78"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F2">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>IF(OR(A2="",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>IF(OR(A2="_ascii",A2="_HEX",A2="_cmd",A2="_dektec"),0,1)</formula>
+    <cfRule type="expression" dxfId="17" priority="2">
+      <formula>IF(OR(A2="_ascii",A2="_cmd",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5538,6 +5466,25 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{C2964006-1830-40A2-88E7-53F888A2750B}">
+            <xm:f>IF(OR(Schedule!A2="_ascii",Schedule!A2="_cmd",Schedule!A2="_dektec"),0,1)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.499984740745262"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H2</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5556,117 +5503,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="96"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-    </row>
-    <row r="5" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+    </row>
+    <row r="5" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="39" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="41" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-    </row>
-    <row r="10" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+    </row>
+    <row r="10" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+    </row>
+    <row r="11" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>